<commit_message>
Added social Media sites
</commit_message>
<xml_diff>
--- a/EnvNP_SG.xlsx
+++ b/EnvNP_SG.xlsx
@@ -543,7 +543,7 @@
       <c r="J2" t="inlineStr"/>
       <c r="K2" t="inlineStr">
         <is>
-          <t>['https://www.facebook.com/naturesocietysingapore/', 'https://www.facebook.com/groups/naturesocietysingapore/', 'https://www.instagram.com/naturesocietysingapore/?hl=en']</t>
+          <t>['https://www.facebook.com/naturesocietysingapore/', 'https://www.instagram.com/naturesocietysingapore/?hl=en', 'https://www.facebook.com/groups/naturesocietysingapore/']</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>['https://www.facebook.com/zerowastesg/', 'https://www.instagram.com/zerowastesingapore/', 'https://sg.linkedin.com/company/zerowastesg']</t>
+          <t>['https://www.facebook.com/zerowastesg/', 'https://sg.linkedin.com/company/zerowastesg']</t>
         </is>
       </c>
     </row>
@@ -1112,7 +1112,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>['https://www.facebook.com/SingaporeEnvironmentCouncil/', 'https://sg.linkedin.com/company/singapore-environment-council', 'https://www.instagram.com/secsingapore/?hl=en', 'https://www.youtube.com/@SECSingapore']</t>
+          <t>['https://sg.linkedin.com/company/singapore-environment-council', 'https://www.instagram.com/secsingapore/?hl=en', 'https://www.facebook.com/SingaporeEnvironmentCouncil/', 'https://www.youtube.com/@SECSingapore']</t>
         </is>
       </c>
     </row>
@@ -1222,7 +1222,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>['https://www.facebook.com/repairkopitiam/', 'https://www.instagram.com/repairkopitiam/?hl=en']</t>
+          <t>['https://www.facebook.com/repairkopitiam/', 'https://www.instagram.com/repairkopitiam/?hl=en', 'https://www.facebook.com/repairkopitiam/photos/']</t>
         </is>
       </c>
     </row>
@@ -1397,7 +1397,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>['https://www.facebook.com/cicadatreeecoplace/', 'https://www.facebook.com/cicadatreeecoplace/photos/']</t>
+          <t>['https://www.facebook.com/cicadatreeecoplace/']</t>
         </is>
       </c>
     </row>
@@ -1448,7 +1448,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['https://www.facebook.com/EarthObservatoryOfSingapore/']</t>
         </is>
       </c>
     </row>
@@ -1504,7 +1504,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>['https://www.facebook.com/groups/greendrinkssingapore/', 'https://www.facebook.com/greendrinkssg/', 'https://www.youtube.com/channel/UCq_vO3-P1ide5sjEJdQAkag']</t>
+          <t>['https://www.facebook.com/groups/greendrinkssingapore/', 'https://www.facebook.com/greendrinkssg/?locale=ps_AF', 'https://www.youtube.com/channel/UCq_vO3-P1ide5sjEJdQAkag']</t>
         </is>
       </c>
     </row>
@@ -1682,7 +1682,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>['https://www.facebook.com/kampung.senang/', 'https://sg.linkedin.com/company/kampungsenang', 'https://www.instagram.com/kampungsenang/']</t>
+          <t>['https://www.facebook.com/kampung.senang/', 'https://sg.linkedin.com/company/kampungsenang']</t>
         </is>
       </c>
     </row>
@@ -1848,7 +1848,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>['https://sg.linkedin.com/company/guildasia', 'https://www.facebook.com/guildsg/', 'https://medium.com/@groundupinnovation/about', 'https://www.facebook.com/guildasia/']</t>
+          <t>['https://sg.linkedin.com/company/guildasia', 'https://www.facebook.com/guildsg/', 'https://www.youtube.com/watch?v=wnbMXZ4zuBM', 'https://www.facebook.com/Lionsforge/videos/guild-ground-up-innovation-labs-for-development-%E3%82%AE%E3%83%AB%E3%83%89-%E7%A4%BE%E5%8C%BA%E5%88%9B%E6%96%B0%E4%BC%9A%E9%A6%86-is-here-at-the-impact/491474829116857/', 'https://medium.com/@groundupinnovation/about', 'https://www.facebook.com/guildasia/']</t>
         </is>
       </c>
     </row>
@@ -1960,7 +1960,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>['https://www.facebook.com/TrashHeroSingapore/', 'https://www.instagram.com/wearetrashherosingapore/?hl=en', 'https://www.facebook.com/TrashHeroSingapore/events/', 'https://www.facebook.com/TrashHeroSingapore/videos/1940092789613462/']</t>
+          <t>['https://www.facebook.com/TrashHeroSingapore/', 'https://www.instagram.com/wearetrashherosingapore/', 'https://www.facebook.com/TrashHeroSingapore/events/', 'https://www.facebook.com/TrashHeroSingapore/videos/1940092789613462/']</t>
         </is>
       </c>
     </row>
@@ -2018,7 +2018,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>['https://www.instagram.com/smallchangelastingimpact/', 'https://www.facebook.com/SmallChangeLastingImpact/', 'https://www.linkedin.com/pulse/butterfly-effect-how-small-changes-can-lead-big-impacts-amr-elharony', 'https://medium.com/@contact_28344/the-power-of-social-impact-how-small-actions-can-create-lasting-change-b96cd9a49e55']</t>
+          <t>['https://www.instagram.com/smallchangelastingimpact/', 'https://www.facebook.com/SmallChangeLastingImpact/', 'https://www.linkedin.com/pulse/power-small-actions-creating-meaningful-impact-lasting', 'https://medium.com/@contact_28344/the-power-of-social-impact-how-small-actions-can-create-lasting-change-b96cd9a49e55']</t>
         </is>
       </c>
     </row>
@@ -2227,7 +2227,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>['https://www.instagram.com/teamseagrass/', 'https://www.facebook.com/TeamSeagrass-172603406103907/', 'https://twitter.com/teamseagrass']</t>
+          <t>['https://www.facebook.com/TeamSeagrass-172603406103907/', 'https://www.instagram.com/teamseagrass/', 'https://twitter.com/teamseagrass', 'https://www.flickr.com/groups/1047086@N21/']</t>
         </is>
       </c>
     </row>
@@ -2498,7 +2498,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>['https://www.facebook.com/ACRESasia/', 'https://sg.linkedin.com/company/acressg']</t>
+          <t>['https://www.facebook.com/ACRESasia/', 'https://sg.linkedin.com/company/acressg', 'https://www.facebook.com/ACRESasia/photos/']</t>
         </is>
       </c>
     </row>
@@ -2611,7 +2611,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>['https://www.facebook.com/groups/sgfoodrescue/', 'https://www.instagram.com/sgfoodrescue/?hl=en', 'https://www.facebook.com/foodrescuesingapore/']</t>
+          <t>['https://www.facebook.com/groups/sgfoodrescue/', 'https://www.facebook.com/foodrescuesingapore/', 'https://www.instagram.com/sgfoodrescue/?hl=en']</t>
         </is>
       </c>
     </row>
@@ -2732,7 +2732,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>['https://sg.linkedin.com/company/eco-sim', 'https://www.instagram.com/ecosim_/', 'https://www.facebook.com/EcoSIMClub/']</t>
+          <t>['https://sg.linkedin.com/company/eco-sim', 'https://www.facebook.com/EcoSIMClub/']</t>
         </is>
       </c>
     </row>
@@ -2786,7 +2786,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>['https://sg.linkedin.com/company/elsa-nuslaw', 'https://www.instagram.com/nuslawelsa/', 'https://www.facebook.com/elsa.nuslaw/', 'https://www.facebook.com/elsaualberta/']</t>
+          <t>['https://sg.linkedin.com/company/elsa-nuslaw', 'https://www.instagram.com/nuslawelsa/', 'https://www.facebook.com/elsa.nuslaw/', 'https://www.facebook.com/elsaualberta/', 'https://www.instagram.com/uottawaelsa/?hl=en']</t>
         </is>
       </c>
     </row>
@@ -2838,7 +2838,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>['https://www.facebook.com/nusvege/', 'https://www.instagram.com/p/CMtnRJll-wg/']</t>
+          <t>['https://www.facebook.com/nusvege/', 'https://www.instagram.com/nusvege/?hl=en']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Test Dataset LLM Model v1
</commit_message>
<xml_diff>
--- a/EnvNP_SG.xlsx
+++ b/EnvNP_SG.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:O43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -434,74 +434,92 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Name of organisation</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Description of organisation</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Mission/ Objectives/ Purpose</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Programmes/ projects</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>Funding sources</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>Collaboration with government / businesses</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Choice of Climate action</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>No. of employees</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>Geographical focus</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>Nationality</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Social Medias</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Top Google Links</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>New_Description</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>LLM_Extracted_Text</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>Nature Society Singapore (NSS)</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="C2" t="inlineStr">
         <is>
           <t>The Nature Society (Singapore) or NSS is a non-government, non-profit organisation dedicated to the appreciation, conservation, study and enjoyment of the natural heritage in Singapore, Malaysia and the surrounding region. It was formerly known as the Singapore branch of the Malayan Nature Society. The branch was formed in 1954 and became Nature Society (Singapore) in 1991.</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="D2" t="inlineStr">
         <is>
           <t>- Organise nature appreciation activities like guided nature walks, bird and butterfly watching, slide talks and overseas eco-trips.
 - Conduct conservation projects and surveys.
@@ -509,7 +527,7 @@
 - Campaign for the protection of natural habitats.</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>- guided nature walks, bird and butterfly watching
 - workshops and courses
@@ -517,54 +535,72 @@
 - various environmental and conservation projects.</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>Run by volunteers, the Society depends financially on contributions from its members as well as companies, institutions and individuals.</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="G2" t="inlineStr">
         <is>
           <t>Yes -  businesses</t>
         </is>
       </c>
-      <c r="G2" t="inlineStr">
+      <c r="H2" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H2" t="n">
+      <c r="I2" t="n">
         <v>43</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>Singapore, Singapore</t>
         </is>
       </c>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr">
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr">
         <is>
           <t>['https://www.facebook.com/naturesocietysingapore/', 'https://www.instagram.com/naturesocietysingapore/?hl=en', 'https://www.facebook.com/groups/naturesocietysingapore/']</t>
         </is>
       </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>['https://www.nss.org.sg/', 'https://en.wikipedia.org/wiki/Nature_Society_(Singapore)', 'https://www.nlb.gov.sg/main/article-detail?cmsuuid=9aa5811a-2a84-440a-b7da-9eb8c88557a6']</t>
+        </is>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t xml:space="preserve">   
+ 	Nature Society (Singapore)
+       Home Facebook RSS  Register Contact Us          News  News Press Release Nature News Events and Calendar Event Payment   Resources  Nature Watch Magazine Publications and Reports Forum Gallery Species Chec    Nature Society (Singapore) - Wikipedia                           Jump to content        Main menu      Main menu move to sidebar hide    		Navigation 	   Main pageContentsCurrent eventsRandom articleAbout WikipediaContact usDonate      		Contribute 	   HelpLearn to editCommunity portalRecent changesUpload file      Languages  Language links are at the top of the page.                    Search            Search                              Create account  Log in         Personal tools       Create account Log in      		Pages for logged out editors learn more    ContributionsTalk                             Contents move to sidebar hide     (Top)      1History        2Major conservation issues    Toggle Major conservation issues subsection      2.1Sungei Buloh        2.2Lower Peirce        2.3Chek Jawa        2.4Kranji Marshes Park        2.5The Green Corridor          3Committees    Toggle Committees subsection      3.1Conservation Committee        3.2Education Committee          4Special interest groups    Toggle Special interest groups subsection      4.1Bird Group        4.2Butterfly &amp; Insect Group        4.3Jalan Hijau        4.4Marine Conservation Group        4.5Plant Group        4.6Vertebrate Study Group          5Former special in    Nature Society (Singapore)                                                (current)          What would you like to find?   Search   Search:   
+                                             {{searchLocationDisplayName}}     Catalogue    OneSearch    Within This Site      Catalogue    OneSearch    Search Within This Site           
+                                     Discover and Learn
+                                                  Discover and Learn   Discover Our Collections  Explore Singapore Collections  Learn          Find Good Reads Find books, journals, magazines, CDs or DVDs.   OneSearch Search through the databases of various libraries and archives, including our partners'.   Subscribed Databases Discover more from various databases including EBSCO, EIU, JStor and others.   Resource Guides Discover topics on Singapore, Arts, Business </t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>WWF Singapore</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="C3" t="inlineStr">
         <is>
           <t>WWF-Singapore was founded in March 2006 to engage individuals and organisations in Singapore towards making a positive change in their lives and business operations.
 Through awareness campaigns and outreach activities, WWF(S) aims to educate individuals from all walks of life on how a simple action can add up to make a big difference to our environment and safeguard the world’s biodiversity.</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>SUSTAIN THE NATURAL WORLD FOR THE BENEFIT OF PEOPLE AND NATURE</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t xml:space="preserve">Climate: Net-zero carbon &amp; Sustainable finance
 Sustainability and Circular economy: Sustainable palm oil &amp; Circular economy 
@@ -573,7 +609,7 @@
 </t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>- Donations from individuals
 - Major donors 
@@ -585,40 +621,53 @@
 - Others</t>
         </is>
       </c>
-      <c r="F3" t="inlineStr">
+      <c r="G3" t="inlineStr">
         <is>
           <t>Yes -  businesses</t>
         </is>
       </c>
-      <c r="G3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H3" t="inlineStr">
+      <c r="I3" t="inlineStr">
         <is>
           <t>39+</t>
         </is>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>Singapore, Singapore</t>
         </is>
       </c>
-      <c r="J3" t="inlineStr"/>
-      <c r="K3" t="inlineStr">
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr">
         <is>
           <t>['https://www.facebook.com/wwfsg/', 'https://www.instagram.com/wwfsg/?hl=en', 'https://sg.linkedin.com/company/wwfsg']</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>['https://www.wwf.sg/', 'https://wwf.panda.org/wwf_offices/singapore', 'https://www.businesstimes.com.sg/companies-markets/wwf-singapore-appoints-vivek-kumar-succeed-outgoing-ceo']</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t xml:space="preserve">WWF-Singapore | Home                                 Skip to content  HomeOur WorkOur WorkClimateNet Zero CarbonSustainable FinanceSustainability &amp; Circular EconomySustainable Palm OilCircular EconomyNature &amp; BiodiversityIllegal Wildlife TradeMarine ConservationForest Landscape RestorationCloser to HomeFuture Sustainability LeadersGreen CitiesAbout UsAbout usChairman &amp; CEO MessageBoard of DirectorsSenior ManagementWhistleblowing PolicyPersonal Data Protection PolicyWork With UsVolunteeringResourcesResourcesAnnual ReportsNews &amp; EventsPartnershipsPartnershipsCorporate PartnershipsGovernment Partnerships  MenuHomeOur WorkOur WorkClimateNet Zero CarbonSustainable FinanceSustainability &amp; Circular EconomySustainable Palm OilCircular EconomyNature &amp; BiodiversityIllegal Wildlife TradeMarine ConservationForest Landscape RestorationCloser to HomeFuture Sustainability LeadersGreen CitiesAbout UsAbout usChairman &amp; CEO MessageBoard of DirectorsSenior ManagementWhistleblowing PolicyPersonal Data Protection PolicyWork With UsVolunteeringResourcesResourcesAnnual ReportsNews &amp; EventsPartnershipsPartnershipsCorporate PartnershipsGovernment Partnerships      MenuSupport WWFDonateAdoptFundraiser  MenuSupport WWFDonateAdoptFundraiser   HomeOur WorkOur WorkClimateNet Zero CarbonSustainable FinanceSustainability &amp; Circular EconomySustainable Palm OilCircular EconomyNature &amp; BiodiversityIllegal Wildlife TradeMarine ConservationForest Landscape RestorationCloser to HomeFuture Sustainability LeadersGreen CitiesAbout UsAbout usChairman &amp; CEO MessageBoard of DirectorsSenior ManagementWhistleblowing PolicyPersonal Data Protection PolicyWork With UsVolunteeri   WWF Singapore office | WWF                                                     We use cookies to analyse how visitors use our website and to help us provide the best possible experience for users. View our Cookie Policy. (I accept)        Archive Content Please note: This page has been archived and its content may no longer be up-to-date. This version of the page will remain live for reference purposes as we work to update the content across our website.         Toggle navigation         Discover     Climate &amp; Energy   Food   Forests   Freshwater   Oceans   Wildlife   People &amp; conservation   More on our work   Knowledge Hub   About WWF      Act     Donate to WWF   Take Action   Partner With WWF   Plastic Pollution Treaty   Subsc  </t>
+        </is>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>Zero Waste SG</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="C4" t="inlineStr">
         <is>
           <t>Zero Waste SG is a charity and non-governmental organisation leading the drive towards zero waste in Singapore through education and advocacy.
 Zero Waste SG started as a website in 2008 providing tips and resources on waste minimisation and recycling.
@@ -626,7 +675,7 @@
 Today, Zero Waste SG has grown to become a recognised charity that has reached over 55,000 people and engaged more than 220 companies through its campaigns and services.</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="D4" t="inlineStr">
         <is>
           <t>Leading the drive towards zero waste in Singapore: Zero Waste SG focuses on engaging the public and corporates on the 3Rs (Reduce, Reuse and Recycle) in areas of:
 1. Food Waste
@@ -635,7 +684,7 @@
 4. Organisational Waste</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>1. BYO Singapore
 2. Zero Waste School
@@ -643,7 +692,7 @@
 4. Save food cut waste</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>1. Donations
 2. Coporate funding
@@ -653,47 +702,60 @@
 6. Others</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G4" t="inlineStr">
         <is>
           <t>Yes -  businesses and government agencies</t>
         </is>
       </c>
-      <c r="G4" t="inlineStr">
+      <c r="H4" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H4" t="n">
+      <c r="I4" t="n">
         <v>9</v>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>Singapore, Singapore</t>
         </is>
       </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K4" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/zerowastesg/', 'https://sg.linkedin.com/company/zerowastesg']</t>
         </is>
       </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>['http://www.zerowastesg.com/', 'https://www.towardszerowaste.sg/', 'https://www.towardszerowaste.sg/zero-waste-nation/']</t>
+        </is>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">        Zero Waste SG – Leading the drive towards zero waste in Singapore                                                                               Zero Waste SGLeading the drive to            Towards Zero Waste Singapore                             A Singapore Government Agency Website                                         How to identify                               Official website links end with .gov.sg                  Government agencies communicate via                  .gov.sg                  websites (e.g. go.gov.sg/open).                                    Trusted websites        Secure websites use HTTPS                  Look for a                  lock () or https:// as an added precaution. Share sensitive                 information only on official, secure websites.                                                Zero Waste Masterplan IntroductionForewordChapter 1 - Towards a Zero Waste NationChapter 2 - Keeping Our Resources Within A Closed LoopChapter 3 - A Circular Economy Approach To Closing Three Resource LoopsChapter 4 - Optimising Infrastructure For Maximum Resource RecoveryChapter 5 - Transforming The Environmental Services IndustryChapter 6 - Shaping A Greener Future With Science And TechnologyChapter 7 - Towards A Zero Waste Nation, Together   Our Foc            Zero Waste Nation                             A Singapore Government Agency Website                                         How to identify                               Official website links end with .gov.sg                  Government agencies communicate via                  .gov.sg                  websites (e.g. go.gov.sg/open).                                    Trusted websites        Secure websites use HTTPS                  Look for a                  lock () or https:// as an added precaution. Share sensitive                 information only on official, secure websites.                                                Zero Waste Masterplan IntroductionForewordChapter 1 - Towards a Zero Waste NationChapter 2 - Keeping Our Resources Within A Closed LoopChapter 3 - A Circular Economy Approach To Closing Three Resource LoopsChapter 4 - Optimising Infrastructure For Maximum Resource RecoveryChapter 5 - Transforming The Environmental Services IndustryChapter 6 - Shaping A Greener Future With Science And TechnologyChapter 7 - Towards A Zero Waste Nation, Together   O</t>
+        </is>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>PM.Haze</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="C5" t="inlineStr">
         <is>
           <t>People’s Movement to Stop Haze, known as PM Haze, is a non-profit focusing on outreach, research and advocacy on the transboundary haze crisis. Our mission is to drive a global movement to stop the haze by empowering the community with the knowledge, means and values. Steering consumption patterns towards sustainable palm oil and paper as well as assisting Indonesian and Malaysian farmers to create a sustainable livelihood are two main ways we empower our community.</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="D5" t="inlineStr">
         <is>
           <t xml:space="preserve">Vision: We envision a world where everyone feels responsible for the clean air we all enjoy
 Mission: We empower people with the values, knowledge and means to drive a movement to
@@ -701,7 +763,7 @@
 </t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="E5" t="inlineStr">
         <is>
           <t>1. Haze-Free Foodstand campaign
 2. Instagram collaboration
@@ -712,53 +774,68 @@
 7. Talks, workshops and events</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t xml:space="preserve">PM Haze is financially supported by the Singapore Institute of International Affairs, The David and Lucile Packard Foundation, and other donations from private individuals.
 </t>
         </is>
       </c>
-      <c r="F5" t="inlineStr">
+      <c r="G5" t="inlineStr">
         <is>
           <t>Yes -  businesses and schools</t>
         </is>
       </c>
-      <c r="G5" t="inlineStr">
+      <c r="H5" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H5" t="n">
+      <c r="I5" t="n">
         <v>9</v>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>Singapore, Indonesia, Malaysia</t>
         </is>
       </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K5" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
           <t>['https://sg.linkedin.com/company/pm-haze', 'https://www.facebook.com/pmhaze/', 'https://www.instagram.com/pmhaze/']</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>['https://www.pmhaze.org/', 'https://en.wikipedia.org/wiki/People%27s_Movement_to_Stop_Haze', 'https://www.haze.gov.sg/']</t>
+        </is>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t xml:space="preserve">                                                          HOME | Pmhaze                             top of pageHOMEABOUT USOur StoryManagement &amp; BoardAnnual ReportsPartnersPublicationsHAZE RESPONSE TOOLKITPSITAKE ACTIONSwitch to Haze-Free Palm OilProtect Peatlands, Prevent HazeBe A PartnerBe A VolunteerDONATEClean Air,Resilient Communities: Together Against HazeEmpowering people with the tools, knowledge, and passion to drive th    People's Movement to Stop Haze - Wikipedia                                     Jump to content        Main menu      Main menu move to sidebar hide    		Navigation 	   Main pageContentsCurrent eventsRandom articleAbout WikipediaContact usDonate      		Contribute 	   HelpLearn to editCommunity portalRecent changesUpload file      Languages  Language links are at the top of the page.                    Search            Search                              Create account  Log in         Personal tools       Create account Log in      		Pages for logged out editors learn more    ContributionsTalk                             Contents move to sidebar hide     (Top)      1Aims        2Work    Toggle Work subsection      2.1Campaigns      2.1.12015: We Breathe What We Buy        2.1.22016: Go Haze Free            3References                  Toggle the table of contents        People's Movement to Stop Haze    1 language     العربية  Edit links            ArticleTalk      English                  ReadEditView history        Tools      Tools move to sidebar hide    		Actions 	   Read   
+ 	Haze - The National Environment Agency
+                          Skip to main         A Singapore Government Agency Website                     Voice search Submit search      				Who We Are 			    					Latest Update 				    					Air Quality 				    					Hotspot 				    					Health Advisory 				    					Media 				    				Resources 			    1-hr PM2.5 Readings Readings over the last 24 hours Pollutant Concentrations Historical Readings Portable Air Cleaners Posters                                 SEARCH                                Latest Update           Full Update                  24-hr PSI 1-hr PM2.5      Air Quality        1-hr PM2.5              North      West    Central    East      South    Map Data©2016 Google        24-hr PSI              North      West    Central    East      South    Map Data©2016 Google                 1-hr PM2.5 reading (µg</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>Centre for a Responsible Future</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="C6" t="inlineStr">
         <is>
           <t>The Centre for a Responsible Future (CRF) is a registered non-profit and charity in Singapore. Formerly known as Vegetarian Society Singapore, CRF was born in 1999 and is one of the oldest organizations in Singapore promoting plant-based living.</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="D6" t="inlineStr">
         <is>
           <t>We inspire and support people and organisations in Singapore to 
 - Move towards a plant-based lifestyle
@@ -768,7 +845,7 @@
 - Support growth in plant-based start-ups and businesses</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
+      <c r="E6" t="inlineStr">
         <is>
           <t xml:space="preserve">1. EarthFest
 2. Veganuary
@@ -780,7 +857,7 @@
 8. Business talks and networks </t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>- grants 
 - business membership
@@ -791,52 +868,65 @@
 - Events</t>
         </is>
       </c>
-      <c r="F6" t="inlineStr">
+      <c r="G6" t="inlineStr">
         <is>
           <t>Yes -  businesses</t>
         </is>
       </c>
-      <c r="G6" t="inlineStr">
+      <c r="H6" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H6" t="n">
+      <c r="I6" t="n">
         <v>5</v>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K6" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/crforgsg/', 'https://www.instagram.com/crforgsg/?hl=en', 'https://sg.linkedin.com/company/centre-for-a-responsible-future', 'https://www.youtube.com/c/CentreforaResponsibleFuture']</t>
         </is>
       </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>['https://www.crf.org.sg/', 'https://www.giving.sg/organisation/profile/a647b237-bdb7-409b-a6d5-069c4096e750', 'https://singapores-green-lobang.fandom.com/wiki/Centre_for_a_Responsible_Future']</t>
+        </is>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">        Centre for a Responsible Future                                                   0               Skip to Content                                         About CRF                   Resources                   Initiatives                   Events                   Members                   Veganuary 2024                   Log In                                                        Take Action                        Open Menu Close Menu                                     About CRF                   Resources                   Initiatives                   Events                   Members                   Veganuary 2024                   Log In                                                        Take Action                        Open Menu Close Menu                                 About CRF                             Centre for a Responsible Future | Singapore's Green Lobang Wiki | Fandom                                               Singapore's Green Lobang Wiki       Explore         Main Page      Discuss     All Pages     Community     Interactive Maps     Recent Blog Posts         To Do List       About Us        How to Contribute         View All Organizations        Volunteering Opportunities     View by Activities       Generates Awareness     Policy Proposals     Research     Organizes Free Events     Organizes Paid Events     Organizes Meet-Ups / Exhibitions     Organizes Training / Workshops for Public‏‎     Organizes Training / Workshops for Organisations     Fundraising        View by Cause A-G       Agriculture     Animal Protection     Built Environment Sustainability     Circular Economy‏‎     Climate change     Energy Sector‏‎     Environmental Education‏‎     Food Waste‏‎     Green Finance        View by Cause H-Z       Natural Disasters     Marine Conservation     Nature conservation     Recycling‏‎     Vegetarianism and Veganism‏‎     Waste Management‏‎        View by Type of Organization       Community Organizers     For Profit     Government-affiliated     Non-Profit/Charities/Trusts     Research Institute     School Club/ Society        View by Active/Inactive       Active Organizations     Inactive Organizations            Community        Community Guidelines       Assume Good Faith     Blocking Policy        Blog     Calendar of Events     Feedback     Green Grants/ Funding     Climate Resources       Books     Websit</t>
+        </is>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>Ground-Up Initiative (GUI)</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="C7" t="inlineStr">
         <is>
           <t>Ground-Up Initiative (GUI) is a non-profit society, with a mission to connect people with Nature, Self &amp; Others. By creating a space to nurture connectedness, creativity &amp; risk-taking, we aspire to build a 21st Century Kampung Culture that cultivates holistic solutions for a happier and more sustainable future.</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+      <c r="D7" t="inlineStr">
         <is>
           <t>We aspire to build a 5G society: Gracious, Green, Giving, Grounded and Grateful – a foundation for a 21st Century Kampung Culture that cultivates holistic solutions for a happier and more sustainable future.</t>
         </is>
       </c>
-      <c r="D7" t="inlineStr">
+      <c r="E7" t="inlineStr">
         <is>
           <t>1. Public workshops
 2. Tours
@@ -844,112 +934,168 @@
 4. Corporate programmes.</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>- philanthropic sponsors
 - patronage programme</t>
         </is>
       </c>
-      <c r="F7" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>Yes -  businesses</t>
         </is>
       </c>
-      <c r="G7" t="inlineStr">
+      <c r="H7" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H7" t="n">
+      <c r="I7" t="n">
         <v>19</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K7" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/groundupinitiative/', 'https://www.instagram.com/groundupinitiative/?hl=en', 'https://sg.linkedin.com/company/groundupinitiative', 'https://www.facebook.com/groundupinitiative/events/']</t>
         </is>
       </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>['https://patron.groundupinitiative.org/', 'https://socialarchi.github.io/post/gui/', 'https://www.giving.sg/organisation/profile/d31bd3c1-47c1-429c-be6b-1dc4314f7a38']</t>
+        </is>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    Ground Up Initiative                                       Home   About   Map   Case Studies                        16  Ground Up Initiative         Ground Up Initiative   Project Name: Kampung Kampus  Location: Singapore, Singapore  Date Designed: 2009  Date Completed: In Progress  Size: 26,000 sqm Client: Goverment Organisations, Local Community, Nee Soon Residents, Leadership and Training Groups  Programme: Education  ABOUT Ground Up Initiative Ground-Up Initiative (GUI) is a non-profit community, guided by the spirit of innovation, resilience and grounded leadership to demonstrate urban sustainability.  ABOUT Kampung Kampus Ground-Up Initiative (GUI) is a non-profit community, guided by the spirit of innovation, resilience and grounded leadership to demonstrate urban sustainability. With the power of community, GUI is building Kampung Kampus, a low-carbon footprint community campus, sited on a 2.6 hectares land plot in Yishun, Singapore. Kampung Kampus aims to be a role model in sustainable living and a School of Life; nurturing an eco-conscious community with the mind, the hands and the heart to be stewards of a more sustainable and happier future.      Kampung Kampus   Interview with CAI Bingyu of Ground Up Initiative Interview Transcript Q1: Ever since you joined GUI, how has it affected or improved your life? I appreciate how things come together a lot more. One thing is the government (support).  For instance, GUI has very limited resources, hence we have to do things very differently. In a way that is more creative, and we have to think out of the box and adapt. The situation changes frequently in a social enterprise like ours and I really appreciate what the country leaders are doing. For instance, during the Covid lockdown, operations at Orto had to close and this caused the pests like rats to come over to GUI where they ate all the produce. As such we now have a pest infestation and we had to adapt and improvise to counter against these unforeseen circumstances. It is not easy to run a nation/company well and there are a lot of things to consider. All of these really make me appreciate things more. In GUI, at the start I thought what I’ll be doing could save the world but at the end all I want is to be a better son, a better husband, a better father to my daughter, as well as a better person for this world.  Q2: What is the proce            </t>
+        </is>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>Conservation International Singapore</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="C8" t="inlineStr">
         <is>
           <t>Conservation International’s global mission is to empower people to protect our most fundamental needs, such as food, water, and a stable climate for the benefit of all life on Earth.</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+      <c r="D8" t="inlineStr">
         <is>
           <t>In Singapore, we are providing environmental education, university internships, and direct support to conservation science and research. Additionally, our partnerships with the private and civil sectors encourage environmental responsibility and sustainability.</t>
         </is>
       </c>
-      <c r="D8" t="inlineStr">
+      <c r="E8" t="inlineStr">
         <is>
           <t>1. Environmental education: school programs, virtual learning 
 2. Conservation finance</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>Conservation International Singapore Conservation Trust (CSCT).</t>
         </is>
       </c>
-      <c r="F8" t="inlineStr">
+      <c r="G8" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G8" t="inlineStr">
+      <c r="H8" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H8" t="inlineStr"/>
-      <c r="I8" t="inlineStr">
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K8" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/CISingapore/', 'https://sg.linkedin.com/company/conservation-international-asia-pacific', 'https://www.facebook.com/Conservation.International.Asia.Pacific/']</t>
         </is>
       </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>['https://www.conservation.org/singapore', 'https://www.conservation.org/places/asia-pacific', 'https://www.conservation.org/about/global-offices']</t>
+        </is>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">        
+ 	Conservation International Singapore
+                         Home
+ Programs and Partnerships
+ Conservation Finance
+                       Facebook       Donate  Single donation Monthly donation           
+ Singapore                              Protecting the nature we all rely on for food, fresh water and livelihoods                                  
+ 	Asia-Pacific
+                         Home
+                     Our Work
+ About Us
+ Join Us
+                       Facebook     twitter     YouTube     Instagram     LinkedIn       Subscribe     Please enter a valid email Thank you for joining the CI Community     Donate  Single Donation Monthly Donation            Blog  
+ USA                              Protecting the nature we all rely on for food, fresh water and livelihoods   What    
+                             Stabilizing Our Climate by Protecting and Restoring Nature
+                             Doubling Ocean Protection
+                             Expanding Nature-Positive Economies
+                               How    
+                             Innovations in Science
+                             Innovations in Finance
+                             Partnering with Communities
+                             Working with Governments
+ 	Global Offices
+                         Home
+                     Our Work
+ About Us
+ Join Us
+                       Facebook     twitter     YouTube     Instagram     LinkedIn       Subscribe     Please enter a valid email Thank you for joining the CI Community     Donate  Single Donation Monthly Donation            Blog  
+ USA                              Protecting the nature we all rely on for food, fresh water and livelihoods   What    
+                             Stabilizing Our Climate by Protecting and Restoring Nature
+             </t>
+        </is>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>Singapore Youth for Climate Action</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="C9" t="inlineStr">
         <is>
           <t>SYCA is a community of youths based in Singapore and we have a common goal of taking climate action. Our aim is to empower youths in Singapore to engage in or lead climate action, be it through policy advocacy, community-based initiatives/initiatives involving the community or school projects.</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="D9" t="inlineStr">
         <is>
           <t>To meaningfully engage young people in environment-related volunteerism</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="E9" t="inlineStr">
         <is>
           <t>- educate through movie or book discussions, panel discussions
 - conducting workshops in schools
@@ -958,48 +1104,61 @@
 - post about local environmental events and activities, parliamentary debates</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr">
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G9" t="inlineStr">
+      <c r="H9" t="inlineStr">
         <is>
           <t>Advocacy</t>
         </is>
       </c>
-      <c r="H9" t="n">
+      <c r="I9" t="n">
         <v>3</v>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K9" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/sgyouthclimateaction/', 'https://www.instagram.com/syclimateaction/?hl=en', 'https://twitter.com/syclimateaction?lang=en']</t>
         </is>
       </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>['https://syca.sg/', 'https://syca.sg/about-2/', 'https://www.channelnewsasia.com/singapore/sustainability-development-goals-un-singapore-voluntary-national-review-youths-3629206']</t>
+        </is>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">                                                                 Singapore to emphasise the role youths play in driving climate action as Grace Fu visits UN next week - CNA                    Skip to main content                       Best News Website or Mobile Service  WAN-IFRA Digital Media Awards Worldwide 2022   Best News Website or Mobile Service  Digital Media Awards Worldwide 2022                                Sign In                          Account         My Feed             Search            Hamburger Menu        Close    Top Stories      Singapore     Asia     World      Commentary     Sustainability     Business     Sport       Latest News     Discover          CNA Insider          Watch      Live TV     News Reports     Documentaries &amp; Shows     TV Schedule       Listen      CNA938 Live     Podcasts     Radio Schedule       Special Reports      Singapore Parliament     Mental Health     Interactives       Lifestyle      Entertainment     Women     Wellness     Living     Style &amp; Beauty     Dining     Travel       Luxury      Experiences     Obsessions     People     Remarkable Living        CNA Eyewitness      Send us a news tip       Events &amp; Partnerships     Branded Content      Business Blueprint     Health Matters     The Asian Traveller       Weather      Edition:   Singapore     Asia                   Close              Close    Top Stories      Singapore     Asia     World      Commentary     Sustainability     Business     Sport       Latest News     Discover          CNA Insider          Watch      Live TV     News Reports     Documentaries &amp; Shows     TV Schedule       Listen      CNA938 Live     Podcasts     Radio Schedule       Special Reports      Singapore Parliament     Mental Health     Interactives       Lifestyle      Entertainment     Women     Wellness     Living     Style &amp; Beauty     Dining     Travel       Luxury      Experiences     Obsessions     People     Remarkable Living        CNA Eyewitness      Send us a news tip       Events &amp; Partnerships     Branded Content      Business Blueprint     Health Matters     The Asian Traveller       Weather          Edition:   Singapore     Asia               Search                            Trending Topics              CNA Explains           China           Malaysia           Israel-Hamas war           Snap Insight           Ukraine invasion           Wellness           Billio</t>
+        </is>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>Waterways Watch Society</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>Waterways Watch Society (WWS) is a non-governmental and non-profit environmental organisation, committed to foster appreciation and promote conservation of our environment, especially the waterways in Singapore. Established in 1998 with only 27 members, WWS has grown to about 700 volunteers today, with ages ranging between 5 to 80 years old and with people from all walks of life.</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>To bring people together to love our waters and to inspire stewardship for our environment
 To promote awareness and appreciation for our waters and environment
@@ -1007,7 +1166,7 @@
 To educate people on the importance of individual responsibility and being environmentally conscious on our lifestyle choices in our daily lives</t>
         </is>
       </c>
-      <c r="D10" t="inlineStr">
+      <c r="E10" t="inlineStr">
         <is>
           <t>1. Assembly/ Corporate Talks
 2. River Monster
@@ -1016,52 +1175,65 @@
 5. Coastal clean-ups</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>Corporate Sponsors</t>
         </is>
       </c>
-      <c r="F10" t="inlineStr">
+      <c r="G10" t="inlineStr">
         <is>
           <t>Yes -  businesses and government agencies</t>
         </is>
       </c>
-      <c r="G10" t="inlineStr">
+      <c r="H10" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>19</v>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>Singapore, Water</t>
         </is>
       </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K10" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/waterwayswatchsociety/', 'https://www.instagram.com/waterwayswatchsociety/?hl=en', 'https://sg.linkedin.com/company/waterways-watch-society', 'https://twitter.com/waterwayswatch?lang=en']</t>
         </is>
       </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>['https://www.wws.org.sg/', 'https://benevity.com/resources/waterways-watch-society', '/search?q=Waterways+Watch+Society&amp;sca_esv=be1f4daf33da1a0f&amp;ei=6IS6ZdjzFpSu4-EPnaC14AY&amp;start=10&amp;sa=N']</t>
+        </is>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">        Home - Waterways Watch Society                                                                                             Facebook Instagram You Tube LinkedIn  Search the site           Menu   About Us  About Waterways Watch Society Our History &amp; Accomplishments Board Committee WWS Team Our Constitution Annual Reports &amp; AGM Minutes   Our Programmes  Corporate Talk School Assembly Talks Corporate Team Bonding  Coney Island Discovery Trail (CIDT) Lorong Halus Discovery Trail (LHDT) Camp Enviro-Awareness   Corporate Social Responsibility  Waterways Clean Up Programmes Beach/ Coastal Cle  How Waterways Watch society turns first-time volunteers into life-long advocates                                                                          Nonprofits  Causes Portal Login Nonprofit Solution Register your nonprofit Benevity Community Impact Network Resources for nonprofits              Solutions   Corporate Purpose Employee Engagement Community Investment Customer Engagement By Topic  Disaster &amp; Crisis Relief International Programs   Products   Employee Engagement  Volunteering Micro-Actions Giving Affinity Groups  Community Investment  Grants  Customer Engagement   CI Portal API     Partnerships   Plans Resources  Get Inspired   Client Stories Purpose Heroes  Connect  Community Webinars &amp; Events Benevity Live  Learn  Resources Impact Reports Speaking of Purpose Social Impact Show CSR 101   About us  Why Benevity Careers Partnership Media Trust and Security                                             How Waterways Watch society turns first-time volunteers into life-long advocates   Waterways Watch Society is a nonprofit organization that promotes awareness, protection and appreciation of the water reservoirs in Singapore. Every year, around 8 million tons of plastic ends up in the ocean, the majority of which enters through rivers and coastlines.  The nonprofit’s main mission is to bring people together to clean up the waterways, inspire stewardship for the environment and for people to take ownership of their actions.  How do they do it exactly? They organize fun outdoor activities with a purpose! Volunteers take part in excursions in kayaks or pedal-boats to fish out litter from the waters, and go on walks or bike rides to clean the shores.  We recently spoke to Patrick, one of the coordinators at the organization on how the nonprofit works with corpora</t>
+        </is>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>Singapore Environment Council</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="C11" t="inlineStr">
         <is>
           <t>The Singapore Environment Council (SEC) was established in 1995 as an independently managed, non-profit, non-governmental organisation (NGO). We are the only recognised member of the Global Ecolabelling Network (GEN) in Singapore. The GEN is a non-profit association of leading eco labelling organisation worldwide. In 2018, SEC was granted United Nations Environment Programme (UNEP) accredited environmental NGO status. We influence thinking on sustainability issues and coordinate environmental efforts in Singapore and the region. We are an approved Institution of Public Character (IPC) with tax exemption status to donors.</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+      <c r="D11" t="inlineStr">
         <is>
           <t>To foster lasting environmental and societal values that encourage and achieve environmental sustainability by:
 - Collaborating with people, industries and governments
@@ -1071,7 +1243,7 @@
 - Recognising environmental excellence by individuals and organisations</t>
         </is>
       </c>
-      <c r="D11" t="inlineStr">
+      <c r="E11" t="inlineStr">
         <is>
           <t>- Eco - Certifications
 - Training and Education
@@ -1080,59 +1252,87 @@
 - Green DNA</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t xml:space="preserve">1. Donations 
 2. Sponsorships
 </t>
         </is>
       </c>
-      <c r="F11" t="inlineStr">
+      <c r="G11" t="inlineStr">
         <is>
           <t>Yes -  businesses and government agencies</t>
         </is>
       </c>
-      <c r="G11" t="inlineStr">
+      <c r="H11" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>27</v>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K11" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
           <t>['https://sg.linkedin.com/company/singapore-environment-council', 'https://www.instagram.com/secsingapore/?hl=en', 'https://www.facebook.com/SingaporeEnvironmentCouncil/', 'https://www.youtube.com/@SECSingapore']</t>
         </is>
       </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>['https://www.sec.org.sg/', 'https://www.giving.sg/organisation/profile/be3a71bd-220d-49c8-88dc-5c9955852955', 'https://www.eco-business.com/news/singapore-environment-council-announces-leadership-change-executive-director-replaced-after-short-tenure-of-two-months/']</t>
+        </is>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">              Singapore Environment Council (SEC)                                           About SEC
+                            Overview
+                                    Board of Directors
+                                    SEC Secretariat
+                                    SEC and UN Sustainable Development Goals
+                                    SEC Timeline
+                                      Programmes
+                            Eco - Certifications
+                                    Training and Education
+                                    Environmental Awards
+                                    SGLS and Enhanced SGLS
+                                    GreenDNA
+                                      Media
+                            Press Room
+                                    Annual Reports
+                                    Singapore Environment Council announces leadership change, executive director replaced after short tenure of two months | News | Eco-Business | Asia Pacific                                                                     Menu        Search                English    English   简体中文   Bahasa Indonesia   Bahasa Malaysia            Publish with us   Subscribe       Sign in                                           Search                                Close search bar   Show all news, opinion, videos and press releases matching   →  About Eco-Business    Topics    Tags    Regions    Sustainable Development Goals    Series          Winner | Asian Digital Media Awards 2023        News  Opinion Podcasts Videos EB Studio Press Releases  Events  Jobs Intelligence Topics   SDGs   More+          International Edition   International Asia Pacific China USA Europe              Menu                  News  Opinion Podcasts Videos EB Studio Press Releases  Events  Jobs Research           Subscribe   Sign in               Close menu     Eco-Business  International Edition                                     Search Eco-Business                           Search           Language  English   简体中文   Bahasa Indonesia   Bahasa Malaysia         Edition International Asia Pacific China USA Europe    Sections  Home    News  Show more News      Industry Spotlight   Feature Series   Special Reports   A-Z Tags     Opinion   Podcasts   Videos    About Us  Show more About us     Our Team Join Us Advisory Board Contributors Contact Us Strategi</t>
+        </is>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>PlasticLite</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="C12" t="inlineStr">
         <is>
           <t>is a grassroots volunteer group that raises awareness about the excessive dependence on single-use plastics in our community, alongside other current issues relating to climate change.</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+      <c r="D12" t="inlineStr">
         <is>
           <t>Plastic-Lite Singapore is a volunteer group started in early September 2016 to inspire Singaporeans to adopt an environmentally conscious, plastic-lite lifestyle. We believe in cutting unnecessary waste and emphasize “refuse” as the first step towards sustainability. Other than reducing waste at source, we aim to eventually instill environmental consciousness in all, and impact our linear plastic-use system to be more circular in nature.</t>
         </is>
       </c>
-      <c r="D12" t="inlineStr">
+      <c r="E12" t="inlineStr">
         <is>
           <t>- Bounce Bags, a bag-share point that aims to reduce the usage of single-use plastic bags 
 - No-Straw Tuesdays, where schools and students reduce their plastic consumption 
@@ -1140,110 +1340,136 @@
 - talks and roadshows at schools, communities, corporates, and public events to raise awareness about plastic pollution and what can be done to stop it.</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr"/>
-      <c r="F12" t="inlineStr">
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
         <is>
           <t>Yes -  businesses and government agencies</t>
         </is>
       </c>
-      <c r="G12" t="inlineStr">
+      <c r="H12" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H12" t="n">
+      <c r="I12" t="n">
         <v>7</v>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t xml:space="preserve">Singapore </t>
         </is>
       </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K12" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/SayNoToPlasticsSG/', 'https://www.instagram.com/plasticlitesg/?hl=en', 'https://sg.linkedin.com/company/plasticlite-singapore', 'https://twitter.com/plasticlitesg']</t>
         </is>
       </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>['http://plasticlite.sg/social-media', 'https://singapores-green-lobang.fandom.com/wiki/Plastic-Lite_Singapore', 'http://plasticlite.sg/outreach/corporates']</t>
+        </is>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      Page not found - Plastic-Lite Singapore                                                                                  About FAQs BOUNCE BAGS Outreach   Social Media Schools Past Initiatives Eateries Corporates Events   Let’s Talk Climat    Plastic-Lite Singapore | Singapore's Green Lobang Wiki | Fandom                                               Singapore's Green Lobang Wiki       Explore         Main Page      Discuss     All Pages     Community     Interactive Maps     Recent Blog Posts         To Do List       About Us        How to Contribute         View All Organizations        Volunteering Opportunities     View by Activities       Generates Awareness     Policy Proposals     Research     Organizes Free Events     Organizes Paid Events     Organizes Meet-Ups / Exhibitions     Organizes Training / Workshops for Public‏‎     Organizes Training / Workshops for Organisations     Fundraising        View by Cause A-G       Agriculture     Animal Protection     Built Environment Sustainability     Circular Economy‏‎     Climate change     Energy Sector‏‎     Environmental Education‏‎     Food Waste‏‎     Green Finance        View by Cause H-Z       Natural Disasters     Marine Conservation     Nature conservation     Recycling‏‎     Vegetarianism and Veganism‏‎     Waste Management‏‎        View by Type of Organization       Community Organizers     For Profit     Government-affiliated     Non-Profit/Charities/Trusts     Research Institute     School Club/ Society        View by Active/Inactive       Active Organizations     Inactive Organizations            Community        Community Guidelines       Assume Good Faith     Blocking Policy        Blog     Calendar of Events     Feedback     Green Grants/ Funding     Climate Resources       Books     Websites     Films, Documentaries, Videos     Podcasts     Social Media        Climate Topics                         FANDOM               				Fan Central			  					BETA				         				Games			         				Anime			         				Movies			         				TV			         				Video			          					Wikis				      								Explore Wikis							    								Community Central				      Page not found - Plastic-Lite Singapore                                                                                  About FAQs BOUNCE BAGS Outreach   Social Media Schools Past Initiatives Eateries Corporates Events   Let’s Talk Clima</t>
+        </is>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>Repair Kopitiam</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>Repairkopitiam operates as a community repair meetup on the last sunday of the month. Members of the public join us designted areas to repair items that range from broken electrical appliances to torn clothing to damaged furniture. By doing so, you engage in responsible e-waste disposal through the guidance of our volunteer Repair Coaches.
 Apart from this, Repair Kopitiam also brings the repair spirit to your community through various courses and activities. Contact us for more!
 This initiative is powered by Sustainable Living Lab, and is part of the Sustainable Singapore Blueprint 2015.</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Repair kopitiam is an initiative to bring the community together through repair so as to combat the throw away culture for a sustainable world.
 We aim to equip individuals from all walks of life with repair skills to bring their items back to life!</t>
         </is>
       </c>
-      <c r="D13" t="inlineStr">
+      <c r="E13" t="inlineStr">
         <is>
           <t>Repairing courses and activities</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>Sustainable Living Lab</t>
         </is>
       </c>
-      <c r="F13" t="inlineStr">
+      <c r="G13" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G13" t="inlineStr">
+      <c r="H13" t="inlineStr">
         <is>
           <t xml:space="preserve">Change to lifestyle </t>
         </is>
       </c>
-      <c r="H13" t="inlineStr"/>
-      <c r="I13" t="inlineStr">
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K13" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/repairkopitiam/', 'https://www.instagram.com/repairkopitiam/?hl=en', 'https://www.facebook.com/repairkopitiam/photos/']</t>
         </is>
       </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>['https://repairkopitiam.sg/', 'https://cityofgood.sg/articles/repair-kopitiam/', 'https://www.ourbetterworld.org/series/environment/story/spoilt-dont-throw-repair']</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">       Repairkopitiam | Love your barang?Fix your barang!                Sign In  Open main menu         Home   About   DIY   Volunteer   FAQ   Event          Want to learn to fix your stuff? Book Event Next Event: 25 Feb 2024, Sun Booking Starts:  9 Feb 12 noon - 21 Feb     What items can you learn to fix?    Electric Repair     Is your oven tripping?      Is your iron wire frayed?      Has your fan stopped working?   Learn to dRepair Kopitiam: Spoilt? Don’t Throw… Repair!  Skip to main content Sign up for our newsletterSign up for our newsletter  search Follow us                                            Donate to OBWSign up / Sign inSign in  What Are You Looking For?    Popular KeywordsEnvironment Women safetyChildhood traumaWildlifeEducationHelping othersMaking an impact You Might Be Interested In View All  Activity These are HER stories   Activity Volunteer Stories: From Hours to Impact   Main navigation Discover Stories  All Stories       Series      Environment Women Mental Health Wildlife Refugees Disabilities Singapore Travel  Community Blogs      Our Stories   Stories of good across 10 different causes  Our Series   It takes more than one story to see the full picture. Explore our Series for multiple perspectives on a single theme.   Our Better Earth   The earth is in danger, but we can still save it if we act now. In our new environmental series, we share what we can do to save our only home.   Empower HER   All women deserve to live in a world that prioritises their safety, voices, and autonomy. Our Better World explores the challenges faced by women and girls across Asia, and seeks to inspire collective action towards creating a better world for them   Silent No More - Giving Voice To Mental Health   Stigma stops us from getting help or helping others. This series explores how we as a community can give ourselves and each other the support we need.   A Wild Life   When communities come together to protect threatened wildlife, it creates a better world where both wildlife and people can thrive.   Refugees: Displaced, Not Discouraged   Dive into the lives of refugees in Asia and how they find ways to thrive against the odds, as well as the communities helping them.   In A Different Sense   Three immersive journeys of disability and inclusion.   From Singapore, With Love   Stories of Singaporeans who see the needs of our international friends and </t>
+        </is>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>Foodscape Collective</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="C14" t="inlineStr">
         <is>
           <t>The Foodscape Collective Ecosystem is a network of individuals, communities, organisations and businesses that come together to support a circulation of energy for a regenerative and sustainable way of living for the self, society and the planet.</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+      <c r="D14" t="inlineStr">
         <is>
           <t>Our mission is to co-create a fair and inclusive circular food system for all.
 We work together to create communities and livelihoods through collaborative and supportive practices.</t>
         </is>
       </c>
-      <c r="D14" t="inlineStr">
+      <c r="E14" t="inlineStr">
         <is>
           <t>gardening and composting workshops
 sustainable food catering consultancy
@@ -1252,59 +1478,72 @@
 research consultancy.</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>exploring co-budgeting in financial support, and value circulation in in-kind support with time, skills and knowledge</t>
         </is>
       </c>
-      <c r="F14" t="inlineStr">
+      <c r="G14" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G14" t="inlineStr">
+      <c r="H14" t="inlineStr">
         <is>
           <t xml:space="preserve">Change to lifestyle </t>
         </is>
       </c>
-      <c r="H14" t="n">
+      <c r="I14" t="n">
         <v>13</v>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K14" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/FoodscapeCollective/', 'https://www.instagram.com/foodscapecollective/', 'https://www.facebook.com/groups/foodscapecollective/']</t>
         </is>
       </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>['https://foodscapecollective.com/', 'https://cityofgood.sg/articles/foodscape-collective/', 'https://foodscapepages.org/']</t>
+        </is>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">        Foodscape Collective – A fair and inclusive circular food system through community-building, education, well-being and research.                                               Menu   About Community Ventures Happenings Support Foodscape Pages                                          About Community Ventures Happenings Support Foodscape Pages                A fair and inclusive circular food system for all.Foodscape Collective    Practices &amp; Values     Our mission is to co-create a fair and inclusive circular food system for all. We work together to create communities and livelihoods through collaborative and supportive practices.          Community-Building         Well-Being         Research         Education           Through the four pods of Education, Well-being, Research and Community-Building, we harness the processes of bringing awareness, integration, regeneration and transformation to our individual and collective journeys.       Join the Foodscape Collective Ecosystem  The Foodscape Collective Ecosystem is a network of individuals, communities, organiFoodscape PagesArticlesThe SauceAboutGet InvolvedArticlesThe SauceAboutGet Involveddefending our landsDefending our lands: Stacking well-tilled soil with food forests for defence agricultureAn opinion piece highlighting Singapore's agricultural past and potential for a food forest as food security in a natural tropical rainforest.Continue readingdefending our landsDefending our lands: Stacking well-tilled soil with food forests for defence agricultureAn opinion piece highlighting Singapore's agricultural past and potential for a food forest as food security in a natural tropical rainforest.Continue readingSG Food Farm StoryLocal Food Systems and Climate ChangeCheck out this series of photo essays featuring five local food growers greening up our urban landscape with their hands in soil, building communities, tackling climate change and food resilience at the same time!Read it hereSG Food Farm StoryLocal Food Systems and Climate ChangeCheck out this series of photo essays featuring five local food growers greening up our urban landscape with their hands in soil, building communities, tackling climate change and food resilience at the same time!Read it herefeaturedLanding on a new pageWelcome to the redesigned Foodscape Pages! We have a new online space, and we'd like to mark this milestone with a</t>
+        </is>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>LepakInSg</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="C15" t="inlineStr">
         <is>
           <t>LepakInSG is an informal environmental group – with the keyword being informal!
 We run an online calendar of environmental events, while working towards a world where Singapore does its fair share to limit global temperature rise to 1.5 degrees, where Singapore limits consumption of resources to what the Earth can regenerate in a year, and where Singapore reduces biodiversity loss to as low as reasonably practical.</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="D15" t="inlineStr">
         <is>
           <t>To (a) be an activist group that pushes Singapore to rethink its current environmental commitments and rethink how things can be done to achieve environmental sustainability in Singapore in 3 areas: climate change, waste, and biodiversity, and
 (b) increase the reach &amp; accessibility of environmental events in SG via a one-stop community-powered calendar.</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="E15" t="inlineStr">
         <is>
           <t>- PublicAction in 2018 and 2021, 
 - Sea Our Shores in 2018
@@ -1312,56 +1551,69 @@
 - Our Wild Spaces in 2021.</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr"/>
-      <c r="F15" t="inlineStr">
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="H15" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H15" t="n">
+      <c r="I15" t="n">
         <v>5</v>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K15" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
           <t>['https://www.instagram.com/lepakinsg/?hl=en', 'https://www.facebook.com/lepakinsg/', 'https://twitter.com/lepakinsg?lang=en']</t>
         </is>
       </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>['https://lepakinsg.wordpress.com/', 'https://www.greenguide.sg/listing/lepakinsg', 'https://envoicesg.wordpress.com/']</t>
+        </is>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      LepakInSG – A one-stop calendar listing environmental events and activities in Singapore! + We engage in advocacy on environmental issues in Singapore!                                                                                                                      LepakInSG  About LepakInSGOur VolunteersMedia FeaturesContact UsOur WorkFood SustainabilityOur Wild Spaces (Land Use Planning)PublicActionOpen LettersOutreachBlogCommentariesLifestyleFeaturesMiss InformedLepak WithLepak AtLepak FlashbackResourcesEnvironmental Parliamentary QuestionsLepak Kaki DatabaseEcoDrop              LepakInSG is an informal environmental group – with the keyword being informal. Our original reason for existence was to run an online calendar of environmental events, but after doing solely that for a month, we got bored. So we started to organise offline activities to raise action and awareness about various environmental issues!Learn more about who we are and what we stand for here!     📅Calendar of environmental events and activities in Singapore   How to use the calendar Simply click on the event titles for description &amp; copy the links to register for tLepakInSG | Green Guide SGExplore guideContribute a listingAbout Green Guide SGLepakInSGEvents groupGo to we       EnVoice – A voice for the Environment by LepakInSG                                                                                                    Skip to content      					EnVoice				  A voice for the Environment by LepakInSG   Menu Lepak In SG Commentaries Miss Informed Lifestyle Features Lepak Flashback About us             Featured   				Jeanette’s Speech at SG Climate Rally 2021: The People in Crisis 4/12/2021			  Hi, my name is Jeanette and I go by she/ her pronouns. I am a student, sister, daughter, volunteer with LepakInSG, and most of all, a resident of our Planet Earth.  For the past 23 years of my life, I’ve experienced many different events like the increasingly intense weather events and progressively unbearable heat in…  Read More        Featured   				Xiang Tian’s Speech at SG Climate Rally 21/9/2019			  Hi, my name is Xiang Tian.   In the environmental community, I’m known as the person who wears slippers and shorts everywhere I go. And I suspect that as temperatures rise in Singapore, more of you will join me.  It might seem funny now, but I doubt we will be laughing when temperatures h</t>
+        </is>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>Cicada Tree Eco-Place</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>The society was formed in urgent response to the alarming climate change crisis and its impact on wildlife and humans. It advocates for the protection of our precious natural heritage and seeks to educate the youth and communities about eco-living to combat global warming.
 To make a difference for wildlife, we have dedicated our efforts to building bridges between the public and our spectacular biodiversity. With this in mind, we champion environmentally-friendly practices that are both impactful and practical, to individuals and organisations alike.</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>1 – To provide affordable and quality environmental education for all, especially the young
 2 – To conserve and protect our natural heritage by raising awareness of both local and regional flora and fauna
 3 – To demonstrate and encourage adoption of an eco-lifestyle by individuals and organisations</t>
         </is>
       </c>
-      <c r="D16" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t xml:space="preserve">- Nature walks
 - Nature workshops
@@ -1373,154 +1625,193 @@
 </t>
         </is>
       </c>
-      <c r="E16" t="inlineStr"/>
-      <c r="F16" t="inlineStr">
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G16" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H16" t="inlineStr"/>
-      <c r="I16" t="inlineStr">
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K16" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/cicadatreeecoplace/']</t>
         </is>
       </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>['https://cicadatree.org.sg/', 'https://www.greenguide.sg/listing/cicada-tree-eco-place', 'https://singapores-green-lobang.fandom.com/wiki/Cicada_Tree_Eco-place']</t>
+        </is>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>Cicada Tree Eco-Place | Green Guide SGExplore guideContribute a listingAbout Green Guide SGCicada Tree Eco-PlaceGo to websiteOverviewCicada Tree Eco-Place is a non    Cicada Tree Eco-place | Singapore's Green Lobang Wiki | Fandom                                               Singapore's Green Lobang Wiki       Explore         Main Page      Discuss     All Pages     Community     Interactive Maps     Recent Blog Posts         To Do List       About Us        How to Contribute         View All Organizations        Volunteering Opportunities     View by Activities       Generates Awareness     Policy Proposals     Research     Organizes Free Events     Organizes Paid Events     Organizes Meet-Ups / Exhibitions     Organizes Training / Workshops for Public‏‎     Organizes Training / Workshops for Organisations     Fundraising        View by Cause A-G       Agriculture     Animal Protection     Built Environment Sustainability     Circular Economy‏‎     Climate change     Energy Sector‏‎     Environmental Education‏‎     Food Waste‏‎     Green Finance        View by Cause H-Z       Natural Disasters     Marine Conservation     Nature conservation     Recycling‏‎     Vegetarianism and Veganism‏‎     Waste Management‏‎        View by Type of Organization       Community Organizers     For Profit     Government-affiliated     Non-Profit/Charities/Trusts     Research Institute     School Club/ Society        View by Active/Inactive       Active Organizations     Inactive Organizations            Community        Community Guidelines       Assume Good Faith     Blocking Policy        Blog     Calendar of Events     Feedback     Green Grants/ Funding     Climate Resources       Books     Websites     Films, Documentaries, Videos     Podcasts     Social Media        Climate Topics                         FANDOM               				Fan Central			  					BETA				         				Games			         				Anime			         				Movies			         				TV			         				Video			          					Wikis				      								Explore Wikis							    								Community Central							          				Start a Wiki			              	Don't have an account?  	Register   	Sign In          FANDOM               Explore       		Current Wiki	                     				Start a Wiki			               	Don't have an account?  	Register   	Sign In          Advertisement      			Sign In		  			Register		          					Singa</t>
+        </is>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Earth Society</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="C17" t="inlineStr">
         <is>
           <t>Earth Society is a non-profit organization formed by a team of individuals who are passionate about environmental protection. The management committee includes experienced environment activists such as former Green club Teacher-in-charge and former student leaders from NTU Earthlink. We have been studying on Global Warming and Solutions to Climate change since 2008. We based our studies on International reports such as UN reports/ NASA reports/ WWF reports and WWI reports. We share information from our studies freely with schools / companies/ organizations/ NGOs. We strongly believe that when the people are well-informed, many people would make some lifestyle changes to reduce global warming and preserve the food and water resources of the planet.</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+      <c r="D17" t="inlineStr">
         <is>
           <t>To spread environmental awareness on global warming and climate change</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="E17" t="inlineStr">
         <is>
           <t xml:space="preserve">-  conduct FREE Assembly talks/ Seminars on Global Warming (and other environmental matters) in Primary, Secondary schools and Tertiary Institutes.
 - Environment Seminar/ Workshops for companies and organizations.
 - participate actively in environment exhibitions, green forums and eco-events. </t>
         </is>
       </c>
-      <c r="E17" t="inlineStr"/>
-      <c r="F17" t="inlineStr">
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
         <is>
           <t>Yes -  businesses</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="H17" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H17" t="inlineStr"/>
-      <c r="I17" t="inlineStr">
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr">
         <is>
           <t>SINGAPORE</t>
         </is>
       </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K17" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/EarthObservatoryOfSingapore/']</t>
         </is>
       </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>['https://www.earthsocietysg.com/', 'https://www.greenguide.sg/listing/earth-society', 'https://en.wikipedia.org/wiki/Tiandihui']</t>
+        </is>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t xml:space="preserve">          Earth Society (Singapore)                                             Home Our Activities  Primary Secondary/ITE/Tertiary Institutes Companies/ NGOs   Research Articles  Climate Change Food and Water Resources Environment Others   Gallery Eco-Weblinks Contact Us   Home   About Us Earth Society is a non-profit organization formed by a team of individuals who are passionate about environmental Earth Society | Green Guide SGExplore guideContribute a listingAbou    Tiandihui - Wikipedia                                     Jump to content        Main menu      Main menu move to sidebar hide    		Navigation 	   Main pageContentsCurrent eventsRandom articleAbout WikipediaContact usDonate      		Contribute 	   HelpLearn to editCommunity portalRecent changesUpload file      Languages  Language links are at the top of the page.                    Search            Search                              Create account  Log in         Personal tools       Create account Log in      		Pages for logged out editors learn more    ContributionsTalk                             Contents move to sidebar hide     (Top)      1History        2The Hongmen today    Toggle The Hongmen today subsection      2.1Hong Kong        2.2Taiwan        2.3Mainland China        2.4Canada        2.5Other          3Biographies        4See also        5References        6Further reading        7External links                  Toggle the table of contents        Tiandihui    10 languages     AfrikaansBân-lâm-gúБългарски한국어Bahasa IndonesiaNederlands日本語Tiếng Việt粵語中文  Edit links            ArticleTalk      English                  ReadEditView history        Tools      Tools move to sidebar hide    		Actions 	   ReadEditView history      		General 	   What links hereRelated changesUpload fileSpecial pagesPermanent linkPage informationCite this pageGet shortened URLWikidata item      		Print/export 	   Download as PDFPrintable version      		In other projects 	   Wikimedia Commons                          From Wikipedia, the free encyclopedia   Chinese fraternal organization, currently secular but historically religious and secretive   This article needs additional citations for verification. Please help improve this article by adding citations to reliable sources. Unsourced material may be challenged and removed.Find sources: "Tiandihui" – news · newspapers · books · scholar · JSTOR (May 2009)</t>
+        </is>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="A18" s="1" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>Green Drinks (Singapore)</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="C18" t="inlineStr">
         <is>
           <t>Founded in November 2007, Green Drinks (Singapore) is a registered non-profit environment-focused society that connects the community, including businesses, activists, academia and government, for knowledge sharing and collaboration opportunities. One way we do this is by organising informal talks every month, over drinks!</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>knowledge sharing and collaboration opportunities through environmental networking</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>- discussion panels, documentary screenings and workshops
 - public campaign – a public awareness campaign to push for safer skincare and cosmetics in Singapore</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>Sponsorship</t>
         </is>
       </c>
-      <c r="F18" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>Yes -  businesses</t>
         </is>
       </c>
-      <c r="G18" t="inlineStr">
+      <c r="H18" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H18" t="n">
+      <c r="I18" t="n">
         <v>1</v>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K18" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/groups/greendrinkssingapore/', 'https://www.facebook.com/greendrinkssg/?locale=ps_AF', 'https://www.youtube.com/channel/UCq_vO3-P1ide5sjEJdQAkag']</t>
         </is>
       </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>['https://www.greendrinks.org/Singapore/clist', 'https://sggreendrinks.wordpress.com/', 'https://sggreendrinks.wordpress.com/about/']</t>
+        </is>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t xml:space="preserve">       Green Drinks (Singapore) connects community, businesses, government, academia and NGOs in the environmental space                                                                                              Skip to content        Menu Downloads Past Green Drinks Sessions Upcoming Green Drinks Session Media Partner With Us! About Green Drinks       Green Drinks (Singapore) connects community, businesses, government, academia and NGOs in the environmental space              13- 15 Oct: Green Is The New Black’s Conscious Festival 2023  Published on October 9, 2023October 9, 2023 by OliviaLeave a comment    The Conscious Festival is back for its 6th year with the offerings of talks, workshops, marketplace and also a bootcamp at South Beach. More details below: Immerse yourself in a world of sustainability, connection and wonder alongside thousands of other conscious souls. This two-day immersive event explores the future of technology and living through the lenses of climate, impact and consciousness. A celebration where music, art, talks, and workshops converge to expand our minds and ignite action. The festival is almost zero waste, plant-based, carbon negative, and has a little something for everyone. Conscious living is an inside-out job. We invite you to join us on this journey of self and planetary discovery to celebrate what already exists, expand what’s possible, and leave with a renewed sense of purpose and hope for our future, now. To find out more, visit https://www.theconsciousfestival.com/.      Categories Uncategorized          Cre8 Sustainability Exhibition at Singapore Discovery Centre  Published on September        About Green Drinks                                                                                                        Skip to content        Menu Downloads Past Green Drinks Sessions Upcoming Green Drinks Session Media Partner With Us! About Green Drinks           About Green Drinks   Founded in November 2007, Green Drinks (Singapore) is a registered non-profit environment-focused society that connects the community, including businesses, activists, academia and government, for knowledge sharing and collaboration opportunities. One way we do this is by organising informal talks every month, over drinks! Occasionally, we hold discussion panels, documentary screenings and workshops, to further engage the public and participan</t>
+        </is>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="A19" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>Hemispheres Foundation</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t xml:space="preserve">Hemispheres Foundation is a not for profit/social enterprise run by a team of professionals and volunteers who provide educational programs and information to schools, community and individuals to promote awareness and informed personal actions concerning environmental and health issues.
 </t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>Hemispheres Foundation seeks to connect youth and the community with nature and the natural environment:
 By linking local concerns to broader environmental issues
@@ -1529,7 +1820,7 @@
 Supporting humanitarian and social projects in Vietnam, Cambodia and South Asia.</t>
         </is>
       </c>
-      <c r="D19" t="inlineStr">
+      <c r="E19" t="inlineStr">
         <is>
           <t>- Talks on Environmental and Public Hygiene (SWCDC)
 - Home AWaRE Audit (SECDC)
@@ -1539,111 +1830,137 @@
 - Student Excellence Program (Study Skills)</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr">
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G19" t="inlineStr">
+      <c r="H19" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H19" t="inlineStr"/>
-      <c r="I19" t="inlineStr">
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K19" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/HemispheresFoundation/', 'https://www.linkedin.com/company/hemispheres-foundation?trk=public_profile_volunteering-position_profile-section-card_full-click', 'https://www.instagram.com/hemispheresfoundation/']</t>
         </is>
       </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>['https://www.hemispheresfund.org/', 'https://cityhallsingapore.com/hemispheres-foundation/', 'https://singaporemagazine.sif.org.sg/Stories/Data/Stories/Honouring-Extraordinary-Women_2014Issue4']</t>
+        </is>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t xml:space="preserve">           Honouring Extraordinary Women                                                                         Stories   e-Magazine   Subscribe   Contact Us              Search                                Stories &gt; Honouring Extraordinary Women2014 • Issue 4Honouring Extraordinary Women Environmentalist, entrepreneur, humanitarian, mother, grandmother, author — Ann Phua is all these and more.     VisionsMulti-tasking comes naturally to Ann Phua, founder of Hemispheres Foundation — from championing major causes like protecting the environment and providing education to children, to housing the homeless, providing clean water to villagers and empowering women to make time for their loved ones.    By Swapna Mitter    It was her love for nature that led Ann Phua to set up the Hemispheres Foundation (hemispheresfund.org) in 1996. She had a clear goal in mind — to provide environmental education to children, and through them, educate the larger community.  The foundation, a social enterprise run by a small team of Singaporeans and expatriate professionals in Singapore, has reached out to more than 500,000 children, bringing into focus issues like global warming and environmental waste.  Hemispheres spearheads campaigns in developing nations like Cambodia, Vietnam and Myanmar, with Phua travelling to these countries to spread the message among the locals to be more environmentally conscious.  The indomitable 63-year-old also chairs the International Women’s Federation of Commerce and Industry Singapore (IWFCIS) — a global business network that provides women entrepreneurs access and resources to participate in business and networking opportunities.   Improving Women’s Lot  “In every culture, in every part of the world, women have always multi-tasked, working quietly behind the scenes to improve the lives of their families and the wider community. We want to recognise these unsung heroes — women with guts to follow their passion in business,” says Phua.    “... we hope to inspire other women that they too can be extraordinary.”    In 2012, IWFCIS instituted the Xtraordinary Women Award which recognises and honours women who successfully manage the domestic front while making a mark as entrepreneurs and social activists. Phua says that what makes a woman extraordinary is “selflessness and belief in family values”.  Phua adds that this award is not about self-glo</t>
+        </is>
+      </c>
     </row>
     <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="A20" s="1" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>Jane Goodall Institute (Singapore)</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="C20" t="inlineStr">
         <is>
           <t>The Jane Goodall Institute (JGI) is a global nonprofit focused on inspiring individual action to improve the understanding, welfare and conservation of the environment, its wildlife and to safeguard the planet we all share. JGI Singapore (JGIS) was founded in 2007 to continue Dr. Jane’s work in Singapore.</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+      <c r="D20" t="inlineStr">
         <is>
           <t>Inspire, educate, and activate individuals to make a better world for animals, people and the environment</t>
         </is>
       </c>
-      <c r="D20" t="inlineStr">
+      <c r="E20" t="inlineStr">
         <is>
           <t xml:space="preserve">- global youth outreach programme
 - wildlife and environment programme
 - public outreach and engagements </t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>- Donations
 - Corporate sponsorships</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
+      <c r="G20" t="inlineStr">
         <is>
           <t>Yes -  businesses</t>
         </is>
       </c>
-      <c r="G20" t="inlineStr">
+      <c r="H20" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H20" t="n">
+      <c r="I20" t="n">
         <v>22</v>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K20" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/JaneGoodallSingapore/', 'https://www.instagram.com/janegoodallsg/', 'https://sg.linkedin.com/company/jane-goodall-institute-singapore']</t>
         </is>
       </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>['https://janegoodall.org.sg/', 'https://www.giving.sg/organisation/profile/a2cb0b9d-a96b-4e18-bd67-b1285f6fcf9a', 'https://blogs.ntu.edu.sg/hp3203-2017-03/jgi-in-singapore/']</t>
+        </is>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t xml:space="preserve">         Jane Goodall Institute (Singapore) I Home for the Environment, Animals and Community                                                                                                                         JGIS In The Media The JGIS Network                       About Us  Jane’s Story Our Vision and Mission Meet the Team Primates of Singapore   Our Programmes &amp; Campaigns  Roots &amp; Shoots Wildlife &amp; Environment  Raffles’ Banded Langur Long-tailed Macaque   Public Outreach &amp; Engagement   Upcoming Events Get Involved  Volunteer Opportunities Internship Opportunities Sign Up For Roots &amp; Shoots Ways To Donate   Blog Contact JGIS In The Media The JGIS Network Donate                       About Us  Jane’s Story Our Vision and Mission Meet the Team Primates of Singapore   Our Programmes &amp; Campaigns  Roots &amp; Shoots Wildlife &amp; Environment  Raffles’ Banded Langur Long-tailed Macaque   Public Outreach &amp; Engagement   Upcoming Events Get Involved  Volunteer Opportunities Internship Opportunities Sign Up For Roots &amp; Shoots Ways To Donate   Blog Contact JGIS In The Media The JGIS Network Donate                                                 JGI in Singapore | Jane Goodall                                                                      Menu Skip to content Introduction Threats to Chimpanzees  Bushmeat Hunting and Pet Trade Habitat Loss and Degradation Disease   Life Story  Childhood Experiences and Family Influence Leakey’s Angels   Gombe Stream Study  Groundbreaking research Gombe Stream Research Center   Jane Goodall Institution  Targeting Stakeholders Programmes under JGI  Lake Tanganyika Catchment Reforestation and Education (TACARE) Roots &amp; Shoots Tchimpounga Chimpanzee Rehabilitation Center   JGI in Singapore   Activism  Past and Upcoming Events Social Media: Goodall’s 5th Reason for Hope   Lifestyle and Beliefs  Vegetarian Religion versus Evolution Animals in Research   Works Awards Criticism References About Me    Jane Goodall “If we kill off the wild, then we are killing a part of our souls.”        JGI in Singapore   Founded in 2007, the Jane Goodall Institute Singapore was set up in order to continue building up on Goodall’s legacy and vision in Singapore. The institute carries forth her beliefs about the importance of being pro-active in extending humaneness to all living things, and how this will have a significant impact on the wellbeing of the wo</t>
+        </is>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="A21" s="1" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>Kampung Senang</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="C21" t="inlineStr">
         <is>
           <t>Kampung Senang Charity and Education Foundation (Kampung Senang) is an eco-conscious charity that adopts a holistic approach to supporting a Green &amp; Healthy lifestyle. Promoting care for all people regardless of cultural or religious background through compassion-filled charity programmes and education, we hope to inspire a healthy and environmentally friendly lifestyle for everyone.</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+      <c r="D21" t="inlineStr">
         <is>
           <t>Provide compassionate care for people in need
 Spur adoption of health-enhancing and eco-friendly lifestyles
 Foster harmony within our communities and our planet</t>
         </is>
       </c>
-      <c r="D21" t="inlineStr">
+      <c r="E21" t="inlineStr">
         <is>
           <t>- Compassion Support Scheme
 - Volunteer Development Scheme
@@ -1651,58 +1968,71 @@
 - Organic farm tours</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>- Donations
 - Corporate sponsorships</t>
         </is>
       </c>
-      <c r="F21" t="inlineStr">
+      <c r="G21" t="inlineStr">
         <is>
           <t>Yes -  businesses</t>
         </is>
       </c>
-      <c r="G21" t="inlineStr">
+      <c r="H21" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H21" t="n">
+      <c r="I21" t="n">
         <v>14</v>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K21" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/kampung.senang/', 'https://sg.linkedin.com/company/kampungsenang']</t>
         </is>
       </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>['https://www.kampungsenang.org/', 'https://www.c3a.org.sg/nsavirtualrs/classroom/classroom-details/lifelong-learning/nsa-kampung-senang-charity-education-foundation', 'https://give.asia/campaign/kampungsenang']</t>
+        </is>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      Kampung Senang Charity &amp; Education Foundation                                                                                                         Membership   Sign up   Login   中文      donate                          Donate to us AR  |   FR   |   Newsletter About Us  About Kampung Senang Corporate Governance  Management Committee Financial Reports   Sponsors &amp; Partners Privacy Policy Media  Annual Reports Newsletter   Events  Green &amp; Healthy Festival  Charity Gala Dinner   Green &amp; Healthy Monday     Our Services  Mobility Aids Holistic Wellness Centre Day Activity Services Organic Farming Tours Student Care Child Care Neurofeedback Services Courses  NSA Courses Wellness Talks Courses/Workshops/Retreats     Our Initiatives  Volunteer Development Scheme  Volunteer Registration   Compassion Support Scheme Green &amp; Healthy Movement Gift of Good Food   Join Us Contact Us Shop                    We Care, We Empower.  We believe that Kampung Senang’s vision of a world of inner peace, harmony, beauty, and unity, where people are inspired to act with gratitude, respect, and unconditional love towards life and nature, can best be realised through a social movement promoting Green and Healthy living. Learn More                    Welcome to Kampung Senang  Kampung Senang Charity and Education Foundation (Kampung Senang) is an eco-conscious charity that adopts a holistic approach to supporting a Green &amp; Healthy lifestyle. Promoting care for all people regardless of cultural or religious background through compassion-filled charity programmes and education, we hope to inspire a healthy and environmentally friendly lifestyle for everyone. more about us              Let Them Speak For Us        Teacher Collene is truly an asset to the school , with her patient, nurturing and understanding demeanour around children. Her teaching strategies are interesting, fun and educational ,making our children look forward to school every day, just so that they get to attend her lessons. They have express            Kampung Senang Charity &amp; Education Foundation                                                                    VirtualRoadshowVirtual Roadshow                                    Home / Classroom / Lifelong Learning / Kampung Senang Charity &amp; Education Foundation				           Kampung Senang Charity &amp; Education    GIVE to Kampung Senang                               </t>
+        </is>
+      </c>
     </row>
     <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="A22" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>Wildlife Conservation Society (Singapore)</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="C22" t="inlineStr">
         <is>
           <t>The Wildlife Conservation Society saves wildlife and wild places worldwide. We do so through science, global conservation, education and the management of the world's largest system of urban wildlife parks, led by the flagship New York Bronx Zoo. Together, these activities change attitudes towards nature and help people imagine wildlife and humans living in harmony. WCS is committed to this mission because it is essential to the integrity of life on Earth. With a commitment to protect 25% of the world’s biodiversity, we address four of the biggest issues facing wildlife and wild places: climate change; natural resource exploitation; the connection between wildlife health and human health; and the sustainable development of human livelihoods.</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="D22" t="inlineStr">
         <is>
           <t>To leverage our resources for greater conservation impact in the Southeast Asia Archipelago Region through strategic partnerships.</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="E22" t="inlineStr">
         <is>
           <t>- PREVENTING SPECIES EXTINCTIONS
 - TACKLING UNSUSTAINABLE (LEGAL) AND ILLEGAL WILDLIFE TRADE
@@ -1712,222 +2042,282 @@
 - UN SUSTAINABLE DEVELOPMENT GOALS</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>- Donations
 - Corporate sponsorships</t>
         </is>
       </c>
-      <c r="F22" t="inlineStr">
+      <c r="G22" t="inlineStr">
         <is>
           <t>Yes -  businesses</t>
         </is>
       </c>
-      <c r="G22" t="inlineStr">
+      <c r="H22" t="inlineStr">
         <is>
           <t>Advocacy/ Mitigation</t>
         </is>
       </c>
-      <c r="H22" t="n">
+      <c r="I22" t="n">
         <v>7</v>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="J22" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K22" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
           <t>['https://medium.com/wcs-conservation-solutions/conservation-and-business-working-together-for-a-sustainable-singapore-6dc14c138d1c']</t>
         </is>
       </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>['https://singapore.wcs.org/', 'https://singapores-green-lobang.fandom.com/wiki/WCS_(Wildlife_Conservation_Society)', 'https://www.glassdoor.sg/Reviews/Wildlife-Conservation-Society-Reviews-E5422.htm']</t>
+        </is>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t xml:space="preserve">        
+ 	WCS Singapore &gt; Home
+                    Skip to main content        
+                 WCS Singapore
+                Menu
+                         Home   About Us   History and Mission   Staff   WCS Singapore in the Southeast Asian Archipelago Region   2020 Strategy   WCS Around the World   News   Contact Us   Work/Volunteer opportunities     Areas of Focus       WCS (Wildlife Conservation Society) | Singapore's Green Lobang Wiki | Fandom                                               Singapore's Green Lobang Wiki       Explore         Main Page      Discuss     All Pages     Community     Interactive Maps     Recent Blog Posts         To Do List       About Us        How to Contribute         View All Organizations        Volunteering Opportunities     View by Activities       Generates Awareness     Policy Proposals     Research     Organizes Free Events     Organizes Paid Events     Organizes Meet-Ups / Exhibitions     Organizes Training / Workshops for Public‏‎     Organizes Training / Workshops for Organisations     Fundraising        View by Cause A-G       Agriculture     Animal Protection     Built Environment Sustainability     Circular Economy‏‎     Climate change     Energy Sector‏‎     Environmental Education‏‎     Food Waste‏‎     Green Finance        View by Cause H-Z       Natural Disasters     Marine Conservation     Nature conservation     Recycling‏‎     Vegetarianism and Veganism‏‎     Waste Management‏‎        View by Type of Organization       Community Organizers     For Profit     Government-affiliated     Non-Profit/Charities/Trusts     Research Institute     School Club/ Society        View by Active/Inactive       Active Organizations     Inactive Organizations            Community        Community Guidelines       Assume Good Faith     Blocking Policy        Blog     Calendar of Events     Feedback     Green Grants/ Funding     Climate Resources       Books     Websites     Films, Documentaries, Videos     Podcasts     Social Media        Climate Topics                         FANDOM               				Fan Central			  					BETA				         				Games			         				Anime			         				Movies			         				TV			         				Video			          					Wikis				      								Explore Wikis							    								Community Central							          				Start a Wiki			              	Don't have an account?  	Register   	Sign In          FA</t>
+        </is>
+      </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" s="1" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
         <is>
           <t>Back to Ground Zero</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>A group that aims to encourage a more environmentally sustainable and conscious lifestyle in Singapore</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>Curate emotional- &amp; eco-literacy programmes for little ones</t>
         </is>
       </c>
-      <c r="D23" t="inlineStr">
+      <c r="E23" t="inlineStr">
         <is>
           <t>Outreach events in Singapore
 Instagram and online posts</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr">
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G23" t="inlineStr">
+      <c r="H23" t="inlineStr">
         <is>
           <t>Adaptation</t>
         </is>
       </c>
-      <c r="H23" t="n">
+      <c r="I23" t="n">
         <v>5</v>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="J23" t="inlineStr">
         <is>
           <t xml:space="preserve">Singapore </t>
         </is>
       </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K23" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/backtogroundzero/', 'https://www.instagram.com/backtogroundzero/?hl=en', 'https://www.quora.com/Why-do-some-people-say-back-to-ground-zero-instead-of-back-to-square-one-and-when-did-this-expression-start-being-used', 'https://www.facebook.com/backtogroundzero/photos/a.887247798352264/1416211172122588/?type=3']</t>
         </is>
       </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>['https://youthactionplan.sg/YACSeason3/teams/back-to-ground-zero/', 'https://www.shopsosu.co/post/interview-back-to-ground-zero', 'https://www.amazon.sg/Back-Ground-Angelo-Thomas-Crapanzano/dp/1640692983']</t>
+        </is>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">                    Meet The Teams                                  Login
+         | 
+         Sign Up  Logout                                                 Backto groundzero                                                                           Problem Statement  Mental health issues are becoming more prevalent in Singapore, particularly amongst the youth. How can we develop preventive measures, and instill stronger emotional regulation, self-awareness and self-care skills from young?    Project Description  backtogroundzero aims to target the gaps in socio-emotional learning among youths in Singapore. The team has developed “Mr Mole’s Mindful Magic”, a series of mindfulness enrichment sessions that use nature and environemental concepts as gateways to help youths develop socio-emotional learning skills.                                 Project By: Chloe Lim, Eunice Aw, Maria Tan                                                     A Few Questions For You           How would you describe your relationship with yourself?     I know myself extremely well    I have a good grasp of my feelings    I occasionally understand why I feel the way I do    I don't understand myself at all!     What mental wellness concepts do you think should be taught to all youths in Singapore?    What is one thing you do that helps you connect with nature and the environment?    How Can We Improve?    Submit        Share this project                     Guest 24/01/22 01:43:25    In response to "How would you describe your relationship with yourself?" I have a good grasp of my feelings          Guest 24/01/22                                                                Interview: An Afternoon with Back To Ground Zero                                         top of pageComplimentary shipping on orders above $50AboutOur BeginningsOur VisionShopMade-to-OrderJournalMoreUse tab to navigate through the menu items.Log InAll PostsSearch3 min readInterview: An Afternoon with B                                                                               Back to Ground Zero : Crapanzano, Angelo Thomas: Amazon.sg: Books                                           Skip to main content           .sg                             Delivering to Singapore 049145                                      Update location                                      All     All Departments Amazon International St</t>
+        </is>
+      </c>
     </row>
     <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>GUILD (Ground-Up Innovation Labs for Development)</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="C24" t="inlineStr">
         <is>
           <t>A citizen invention lab focused on growing grounded innovators through Nature, Technology and Community towards building a more sustainable, resilient and co-creative Asia.</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+      <c r="D24" t="inlineStr">
         <is>
           <t>to grow innovators who care about nature and community – in other words – grounded innovators!</t>
         </is>
       </c>
-      <c r="D24" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>- Design thinking programme
 - Learning journeys
 - invention workshop</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr">
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
         <is>
           <t>Yes - government</t>
         </is>
       </c>
-      <c r="G24" t="inlineStr">
+      <c r="H24" t="inlineStr">
         <is>
           <t>Adaptation</t>
         </is>
       </c>
-      <c r="H24" t="n">
+      <c r="I24" t="n">
         <v>3</v>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="J24" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K24" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
           <t>['https://sg.linkedin.com/company/guildasia', 'https://www.facebook.com/guildsg/', 'https://www.youtube.com/watch?v=wnbMXZ4zuBM', 'https://www.facebook.com/Lionsforge/videos/guild-ground-up-innovation-labs-for-development-%E3%82%AE%E3%83%AB%E3%83%89-%E7%A4%BE%E5%8C%BA%E5%88%9B%E6%96%B0%E4%BC%9A%E9%A6%86-is-here-at-the-impact/491474829116857/', 'https://medium.com/@groundupinnovation/about', 'https://www.facebook.com/guildasia/']</t>
         </is>
       </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>['https://www.groundupinnovation.org/', 'https://glints.com/companies/guild-ground-up-innovation-labs-for-development/09ca9ae6-c7c2-41c8-a347-d4c143aa13f6', 'https://lessonsgowhere.com.sg/lesson-providers/guild-ground-up-innovation-labs-for-development']</t>
+        </is>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">      Ground-Up Innovation Labs for Development – Growing Grounded Innovators                                       
+ 		Skip to content                           Home Experiences About Contact       Search for:   Search         Search                                 Main Menu             Home Experiences About Contact                                 Growing Grounded Innovators     We empower the young and the young-at-heart to create innovative, impactful inventions for nature and community        About Us                      Design Thinking Programmes      We work with schools and other educational institutions to curate DT programmes ranging from 2-day hackathons to mult                            GUILD Ground Up Innovation Labs for Development - Lesson Provider - LessonsGoWhere                     Toggle navigation              Categories Browse AllArtsArt AppreciationCalligraphyDigital ArtDrawingPaintingPhotography &amp; VideographyBakingBread BakingBubble TeaCake BakingCake DecoratingChocolate MakingDessertsGluten Free BakingIce Cream MakingMacaronsPastryChinese Musical InstrumentsDiziErhuGuqinGuzhengPipaCookingChineseCommercial cookingIndianItalianJapaneseLocalThaiVegetarianVietnameseWesternCraftsBookbindingCarpentryClayCraftFlower ArrangementGlass MakingHamper &amp; Gift WrappingJewellery MakingLeather CraftMetalworkingMiniatures PaintingPotteryRecycling/UpcyclingScrapbookingSewingSilkscreen PrintingTerrariumTypographyDanceBalletBallroom DanceBelly DanceContemporary DanceHip HopJazzKPopOthersSalsaTap DanceE-Learning / Online CoursesAcademics (Online Courses)Business (Online Courses)Design (Online Courses)Development (Online Courses)IT &amp; Software (Online Courses)IT &amp; Software - By eduCBA (Online Courses)Marketing (Online Courses)Office Productivity (Online Courses)Personal Development (Online Courses)Photography &amp; Videography (Online Courses)ExoticAstrologyBath SaltCandle MakingGardeningPerfumeSoap MakingTea/Coffee AppreciationWine AppreciationFitnessAqua AerobicsDance-FitnessGroup FitnessParkourPilatesPiloxingYogaZumbaFor KidsArt Classes for KidsBaking Classes for KidsCooking Classes for KidsCraft Classes for KidsDance Classes for KidsEnrichment Classes for KidsCoding &amp; RoboticsFitness Classes for KidsLanguage Classes for KidsMusic Classes for KidsSports Classes for KidsLanguageArabicChineseEnglishFrenchGermanHindiIndonesianItalianJapaneseKoreanLanguageMongo</t>
+        </is>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="A25" s="1" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t xml:space="preserve">Straw Free Singapore        </t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="C25" t="inlineStr">
         <is>
           <t>Straw Free Singapore is a youth driven movement to reduce the number of plastic straws used in Singapore!</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+      <c r="D25" t="inlineStr">
         <is>
           <t>a youth-driven campaign to reduce the number of plastic straws used here</t>
         </is>
       </c>
-      <c r="D25" t="inlineStr">
+      <c r="E25" t="inlineStr">
         <is>
           <t>- talks
 - outreach campaigns</t>
         </is>
       </c>
-      <c r="E25" t="inlineStr"/>
-      <c r="F25" t="inlineStr">
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
         <is>
           <t>Yes - government and businesses</t>
         </is>
       </c>
-      <c r="G25" t="inlineStr">
+      <c r="H25" t="inlineStr">
         <is>
           <t>Mitigation</t>
         </is>
       </c>
-      <c r="H25" t="n">
+      <c r="I25" t="n">
         <v>4</v>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="J25" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K25" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
           <t>['https://www.instagram.com/strawfreesingapore/?hl=en']</t>
         </is>
       </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>['http://www.byosingapore.com/pact-straw-free/', 'https://www.yp.sg/straw-free-sg/', 'https://www.straitstimes.com/singapore/spotted-straw-free-initiatives-at-some-eateries-here-its-all-thanks-to-this-17-year-old']</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">            PACT (Straw-Free) – BYO Singapore                                                                   Primary Menu Campaigns  BYOB 2023   BYO Supporters  Why BYO Resources Stories   How to BYO BYO Container PACT (Straw-Free)  Straw-Free Week 2018   Downloads  Reports               Over 270 F&amp;B outlets in Singaporephase out plastic straws            What is PACT?         Started by WWF-Singapore, PACT (Plastic ACTion) is a voluntary, business initiative to eliminate plastic pollution in nature and towards a circular economy on plastics where no materials are wasted. PACT recognises the integral role that businesses have in the production and consumption of plastics globally, and the need for more accountability for the plastics these businesses introduce into the market.      With growing momentum across the world against plastics, businesses have been looking to take action. However, we need to avoid incomplete or fragmented measures like replacing plastics with materials that can have a higher environmental footprint, or alternatives that might lead to worse environmental outcomes. Under the PACT initiative, WWFs team works with businesses, to provide advice, assistance and helps them take science-based decisions every step of the way. As part of PACT, which is supported by the National Environment Agency and Zero Waste SG, over 270 food and beverage (F&amp;B) outlets in Singapore will phase out plastic straws by 1 July 2019, in a major industry push to reduce the use of plastic disposables. The F&amp;B outlets will remove straws completely from their premises or provide them only on request.   going straw-free by 1 July 2019    A Poke Theory Accor Group (Raffles, Swissotel, Fairmont, SO, Sofitel, Grand Mercure, Novotel, Mercure, Ibis, Ibis Styles) Bettr Barista Brawn &amp; Brains Coffee Carrotsticks &amp; Cravings Foreword Coffee Grand Hyatt Singapore Guzman Y Gomez iFood Pte Ltd (Good News Cafe, Providence Cafe) Jones the Grocer      Kraftwich Lo &amp; Behold (Loof, Over Easy, White Rabbit, Tanjong Beach Club, Rabbit Hole, Extra Virgin Pizza, Black Swan, Odette, Le Bon Funk, Straits Clan, Clan cafe, Esora) Nam Nam Nandos Nylon Coffee Roasters PastaMania Plain Vanilla Bakery Ramada Days SaladStop! SODEXO SunTec Convention Centre      SuperNature (Glow) Tadcaster Hospitality (Cafe Melba, The Exchange, BQ Bar, Molly Malone’s, Bullandbear) The Coffee Academics The Soci</t>
+        </is>
+      </c>
     </row>
     <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="A26" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>Trash Hero Singapore</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="C26" t="inlineStr">
         <is>
           <t>Community volunteer group with the aim of clearing current and preventing future waste through education.</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>The Trash Hero mission is to bring communities together to clean and reduce waste</t>
         </is>
       </c>
-      <c r="D26" t="inlineStr">
+      <c r="E26" t="inlineStr">
         <is>
           <t>- activities and workshops
 - trash clean up
 - long-term programmes that help communities to reduce and better manage existing waste</t>
         </is>
       </c>
-      <c r="E26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>- In-kind donation
 - Donations from local businesses and government organisations
@@ -1935,52 +2325,65 @@
 - Sponsors</t>
         </is>
       </c>
-      <c r="F26" t="inlineStr">
+      <c r="G26" t="inlineStr">
         <is>
           <t>Yes - government and businesses</t>
         </is>
       </c>
-      <c r="G26" t="inlineStr">
+      <c r="H26" t="inlineStr">
         <is>
           <t>Mitigation &amp; Adaptation</t>
         </is>
       </c>
-      <c r="H26" t="n">
+      <c r="I26" t="n">
         <v>8</v>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="J26" t="inlineStr">
         <is>
           <t xml:space="preserve">Singapore </t>
         </is>
       </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K26" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/TrashHeroSingapore/', 'https://www.instagram.com/wearetrashherosingapore/', 'https://www.facebook.com/TrashHeroSingapore/events/', 'https://www.facebook.com/TrashHeroSingapore/videos/1940092789613462/']</t>
         </is>
       </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>['https://trashhero.org/network/trash-hero-singapore/', 'https://trashhero.org/category/trash-hero-singapore/', 'https://www.eventbrite.sg/e/66th-trash-hero-singapore-clean-up-east-coast-beach-area-h-tickets-747923749067']</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t xml:space="preserve">         Trash Hero Singapore - Trash Hero World                                                                                                            ItalianGermanEnglish                    About us Our Mission Our Organisation Board of Trustees Funding Media Kit   Our Programmes Community Cleanups Water Refill Network Kids &amp; Education Trash Hero Communities Partnerships   Our Network Our Impact Success Stories Media Coverage Trash Hero Blog   Donate Join us Start a new chapter Volunteer Job offers   Contact us                             Trash Hero Singapore      Founded: June 2017 Email: singapore@trashhero.org Social Media:                  Note: the best way to contact us is via ou         Trash Hero Singapore - Trash Hero World                                                                                               English                    About us Our Mission Our Organisation Board of Trustees Funding Media Kit   Our Programmes Community Cleanups Water Refill Network Kids &amp; Education Trash Hero Communities Partnerships   Our Network Our Impact Success Stories Media Coverage Trash Hero Blog   Donate Join us Start a new chapter Volunteer Job offers   Contact us                                    Putting volunteers first                                   by                             Seema                                         on            26/06/2019                1 comment       The latest round of Trash Hero Family Meetings drew to a close this week in Zurich, Switzerland. The city was one of two new European locations that hosted our                                                                       66th Trash Hero Singapore Clean Up - East Coast Beach area H Tickets, Sun 19 Nov 2023 at 09:00 | Eventbrite                                  EventbriteEventbriteSearch eventsSearchFind EventsCreate EventsHelp CentreHelp CentreFind your ticketsContact your event organizerLog InSign UpEventbriteEventbriteSearch eventsSearchLog InSign UpFind EventsCreate EventsSolutionsSolutionsEvent TicketingEvent Marketing PlatformEventbrite AdsPaymentsIndustryIndustryMusicFood &amp; BeveragePerforming ArtsCharity &amp; CausesRetailEvent TypesEvent TypesConcertsClasses &amp; WorkshopsFestivals &amp; FairsConferencesCorporate EventsOnline EventsBlogBlogTips &amp; GuidesNews &amp; TrendsCommunityTools &amp; FeaturesCreate EventsContact SalesGet StartedHelp CentreHelp CentreFind your </t>
+        </is>
+      </c>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="A27" s="1" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
           <t>Small Change Lasting Impact</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="C27" t="inlineStr">
         <is>
           <t xml:space="preserve">Small Change is a grassroots organisation working to bring individuals closer to nature. </t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+      <c r="D27" t="inlineStr">
         <is>
           <t xml:space="preserve">We believe that through a deeper and more meaningful connection with our environment, we can all become better guardians of the world around us. </t>
         </is>
       </c>
-      <c r="D27" t="inlineStr">
+      <c r="E27" t="inlineStr">
         <is>
           <t>- beach clean-ups
 - intertidal walks
@@ -1989,159 +2392,201 @@
 - conservation camps</t>
         </is>
       </c>
-      <c r="E27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>- Donations
 - fees from corporate events</t>
         </is>
       </c>
-      <c r="F27" t="inlineStr">
+      <c r="G27" t="inlineStr">
         <is>
           <t>Yes - businesses</t>
         </is>
       </c>
-      <c r="G27" t="inlineStr">
+      <c r="H27" t="inlineStr">
         <is>
           <t>Mitigation/ Advocacy</t>
         </is>
       </c>
-      <c r="H27" t="inlineStr"/>
-      <c r="I27" t="inlineStr">
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K27" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
           <t>['https://www.instagram.com/smallchangelastingimpact/', 'https://www.facebook.com/SmallChangeLastingImpact/', 'https://www.linkedin.com/pulse/power-small-actions-creating-meaningful-impact-lasting', 'https://medium.com/@contact_28344/the-power-of-social-impact-how-small-actions-can-create-lasting-change-b96cd9a49e55']</t>
         </is>
       </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>['https://www.smallchangesg.com/', 'https://www.smallchangesg.com/how-we-work', 'https://justinthomasmiller.com/the-butterfly-effect-small-changes-lead-to-massive-progress/']</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t xml:space="preserve">        Small Change                                                    0                Skip to Content                                      How we work                   Individuals                   Organisations                   Upcoming                   Contact                                                   Support us                        Open Menu Close Menu                                     How we work                   Individuals                   Organisations                   Upcoming                   Contact                                                   Support us                        Open Menu Close Menu                                 How we work                     Individuals                     Organisations                     Upcoming                     Contact                                            Support us                                 We love, therefore we protect.               ExperienceEducate Evoke     Small Change is a grassroots organisation working to bring individuals closer to nature. We believe that through a deeper and more meaningful connection with our environment, we can         How we work — Small Change                                             0                Skip to Content                                      How we work                   Individuals                   Organisations                   Upcoming                   Contact                                                   Support us                        Open Menu Close Menu                                     How we work                   Individuals                   Organisations                   Upcoming                   Contact                                                   Support us                        Open Menu Close Menu                                 How we work                     Individuals                     Organisations                     Upcoming                     Contact                                            Support us                                 Since 2017, Small Change has run over 60 experiences and workshops               Small Change can lead to lasting impact     ExperienceSmall Change organises a broad range of events which help people experience the wonder of the natural world first hand —  often in surprising ecosystems close to home, that may otherwise be overlooked. These exper</t>
+        </is>
+      </c>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="A28" s="1" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
         <is>
           <t>International Coastal Cleanup, Singapore (ICCS)</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="C28" t="inlineStr">
         <is>
           <t>The International Costal Cleanup Singapore is an annual environmental exercise conducted since 1992 by over 3,000 volunteers by more than 50 organisations and schools.</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="D28" t="inlineStr">
         <is>
           <t>The programme aims to remove and collect data on the debris from the shorelines, waterways and beaches of the world's lakes, rivers and oceans. This information serves to educate the public on marine debris issues and to encourage positive change by submissions to governmental and international organisations that will reduce debris in waterways and enhance aquatic environments.</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="E28" t="inlineStr">
         <is>
           <t>- coastal cleanups
 - Educational projects &amp; School Talks</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr"/>
-      <c r="F28" t="inlineStr">
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G28" t="inlineStr">
+      <c r="H28" t="inlineStr">
         <is>
           <t>Adaptation</t>
         </is>
       </c>
-      <c r="H28" t="n">
+      <c r="I28" t="n">
         <v>12</v>
       </c>
-      <c r="I28" t="inlineStr">
+      <c r="J28" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K28" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/iccsg/']</t>
         </is>
       </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>['https://coastalcleanup.nus.edu.sg/', 'https://www.nss.org.sg/project.aspx?id=41', 'http://coastalcleanup.nus.edu.sg/aboutcleanup.html']</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">    International Coastal Cleanup Singapore            International Coastal Cleanup, SingaporeBattling marine trash in Singapore since 1992The 29th International Coastal Cleanup Singaporehas been cancelled        ICCS Home  About the Cleanup  Why cleanup?  Organisers Page  Zones &amp; Sites  Resourc   
+ 	Nature Society (Singapore)
+       Home Facebook RSS  Register Contact Us          News  News Press Release Nature News Events and Calendar Event Payment   Resources  Nature Watch Magazine Publications and Reports Forum Gallery Species Checklist Links   Shop Groups   Bird Group Butterfly &amp; Insect Group Conservation Committee Education Group Jalan Hijau Group Marine Conservation Group Plant Group The Nature Ramblers Vertebrate Study Group   Support Us   Membership  Volunteer Donate Our Sponsors   Activities   Activities for Members   Surveys   PROJECTS   NSS Rewilding Project  NSS Singapore Nature Sightings  Every Singaporean A Naturalist   Raffles’ Banded Langur Working Group   Restore Ubin Mangroves (R.U.M.) Project  Green Corridor Watch  Coastal Clean Up @ Pulau Ubin  Coastal Clean Up @ Kranji Mudflats  International Coastal Cleanup Singapore (ICCS)   Forest Clean Up @ Pulau Ubin  Horseshoe Crab Rescue &amp; Research Programme   Invasive Species Management Programme  Study of Migratory Bird Crash  Birder's Corner  (Birds of Prey) Raptor Records  iNaturalist Singapore Butterflies Project  iNaturalist Singa   International Coastal Cleanup Singapore             International
+            Coastal Cleanup, Singapore         ICCS Home  About the Cleanup  Why cleanup?  Organisers Page  Zones &amp; Sites  Resources   Participants Page  Results &amp; Photos  Coordinators Contact us   Coordinated by: NUS Toddycats         About the International Coastal Cleanup    The International Coastal Cleanup (ICC) is an annual event conducted in 70-100 countries, coordinated by the US-based agency, The Ocean Conservancy, a non-profit organisation. The programme aims to remove and collect data on the debris from the shorelines, waterways and beaches of the world's lakes, rivers and oceans. This information serves to educate the public on marine debris issues and to encourage positive change by submissions to governmental and international organisations that will reduce debris in waterways and enhance aquatic environments. The International Coastal Cleanup, Singapo</t>
+        </is>
+      </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" s="1" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
         <is>
           <t>Love Our Macritchie Forests</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="C29" t="inlineStr">
         <is>
           <t>A campaign started in response to raise awareness about the potential harm the Cross Island Line is likely to cause to one of Singapore's most precious and pristine ecosystems.</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>We hope that by sharing how special MacRitchie Forest is to Singapore, you will find reasons to love it, and lend your voice to save it.</t>
         </is>
       </c>
-      <c r="D29" t="inlineStr">
+      <c r="E29" t="inlineStr">
         <is>
           <t>- free guided “Love MacRitchie” walks monthly</t>
         </is>
       </c>
-      <c r="E29" t="inlineStr"/>
-      <c r="F29" t="inlineStr">
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G29" t="inlineStr">
+      <c r="H29" t="inlineStr">
         <is>
           <t>Mitigation/ Advocacy</t>
         </is>
       </c>
-      <c r="H29" t="n">
+      <c r="I29" t="n">
         <v>3</v>
       </c>
-      <c r="I29" t="inlineStr">
+      <c r="J29" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K29" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/lovemacritchie/']</t>
         </is>
       </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>['https://lovemacritchie.wordpress.com/', 'https://lovemacritchie.wordpress.com/about-main/', 'https://cicadatree.org.sg/conservation/love-our-macritchie-forest/']</t>
+        </is>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t xml:space="preserve">       Love Our MacRitchie Forest – Keep our green heart beating                                                                                                       		Skip to content	         Love Our MacRitchie Forest Keep our green heart beating             Menu	 Why Love MacRitchie    Irreplaceable habitats and biodiversity Forest fragmentation Convention on Biological Diversity A Nature Reserve is a Nature Reserve An alternative is available   Love MacRitchie walks Biodiversity    Fauna Flora   Take action Blog    Love MacRitchie Walks Events Knowledge News   Media    Media Coverage Infographics Short film Music Videos Art installation   About &amp; Contact     			Scroll down to content		                  An upcoming Cross Island MRT Line is slated to pass beneath MacRitchie forest in Singapore’s Central Catchment Nature Reserve, under some of our most pristine ecosystems, such as old regrowth and century-old primary forests. This isn’t right.  Find out more. Cover video:  Love Our MacRitchie Forest Official Music Video. Watch it with audio here.                   We conduct free guided “Love MacRitchie” walks monthly, to explore MacRitchie’s rich biodiversity.   Book yourself on our next walk.            Love MacRitchie Blog        Posted on January 5, 2020January 6, 2020  Lessons from six years of loving MacRitchie   What a ride it has been. After a demon       About – Love Our MacRitchie Forest                                                                                                         		Skip to content	         Love Our MacRitchie Forest Keep our green heart beating             Menu	 Why Love MacRitchie    Irreplaceable habitats and biodiversity Forest fragmentation Convention on Biological Diversity A Nature Reserve is a Nature Reserve An alternative is available   Love MacRitchie walks Biodiversity    Fauna Flora   Take action Blog    Love MacRitchie Walks Events Knowledge News   Media    Media Coverage Infographics Short film Music Videos Art installation   About &amp; Contact             About   The Love MacRitchie movement is a collective effort among various nature groups in Singapore. It was launched in 2013 in response to the LTA’s announcement of the new Cross Island MRT Line (CRL), which was proposed to tunnel through the MacRitchie Forest, a precious yet fragile ecosystem. We hope that by sharing how special MacRitchie Forest is to Si</t>
+        </is>
+      </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="A30" s="1" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
         <is>
           <t>NUS Toddycats</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="C30" t="inlineStr">
         <is>
           <t>NUS Toddycats!  are volunteers with the Lee Kong Chian Natural History Museum and the Department of Biological Sciences at the National University of Singapore. The name is derived form the common name of the common palm civet (Paradoxurus hermaphroditus), one of the last wild carnivorans in urbanised Singapore.</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+      <c r="D30" t="inlineStr">
         <is>
           <t>Toddycats! is meant to expose, develop, enthuse and apply individuals to programmes in conservation, education and research.</t>
         </is>
       </c>
-      <c r="D30" t="inlineStr">
+      <c r="E30" t="inlineStr">
         <is>
           <t>- Exhibitions
 - Nature and heritage trails 
@@ -2151,98 +2596,127 @@
 - Active partnerships with other groups, agencies and institutions on programmes, events and national strategies and action plans that achieve common goals.</t>
         </is>
       </c>
-      <c r="E30" t="inlineStr"/>
-      <c r="F30" t="inlineStr">
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
         <is>
           <t>Yes - governments</t>
         </is>
       </c>
-      <c r="G30" t="inlineStr">
+      <c r="H30" t="inlineStr">
         <is>
           <t>Mitigation/ Advocacy</t>
         </is>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>19</v>
       </c>
-      <c r="I30" t="inlineStr">
+      <c r="J30" t="inlineStr">
         <is>
           <t xml:space="preserve">Singapore </t>
         </is>
       </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K30" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/nustoddycats/', 'https://www.instagram.com/nustoddycats/']</t>
         </is>
       </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>['https://toddycats.wordpress.com/', 'https://lkcnhm.nus.edu.sg/support/volunteer/toddycats/', 'https://www.nus.edu.sg/inside-nus/stories/a-walk-on-nus-wild-side']</t>
+        </is>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t xml:space="preserve">        NUS Toddycats! | Volunteers with the Lee Kong Chian Natural History Museum, National University of Singapore                                                                                                NUS Toddycats!   Volunteers with the Lee Kong Chian Natural History Museum, National University of Singapore   Skip to content Home HOWL 2024 Calendar About Programmes Join Contact Us             ← Older posts    One Million Trees – 25 sessons this year at Rail Corridor South, Lim Chu Kang and Kent Ridge!  Posted on Sunday, 21 January 2024 by otterman | Leave a comment   In this fifth year of the One Million Tree movement, NUS Toddycats, with NParks and NUS, have scheduled at least 25 reforestation sessions (tree-planting and maintenance) from March to November 2024 at:  Rail Corridor South (Ghim Moh) – 10 sessions Cashin House at Lim Chu Kang Nature Park – 10 sessions Kent Ridge in NUS  – 6 sessions  Some 300 saplings were planted at Rail Corridor South in 2023 The 2024 calendar of activities is available at https://toddycats.wordpress.com/2024-calendar/, and the individual registation links will go live two weeks before each event. Alternatively, you are welcome to join the NUS Toddycats Telegram channel for updates at https://t.me/+Qvfk5NM2gPFjZjVl.  The plant species at these long-term reforestation and afforestation sites are specifically selected and care is taken over the soil enhancement, planting techniques and maintenance of the plants. To keep a rein on mortality, we conduct Sapling Protection Action some two weeks after planting and at regular intervals after. Everyone is welcome to get out into nature for a meaningful activity amidst growing forests with friends and family, and to actively support the SGP2030 vision of a City in Nature. Here’s to a nurtuting new year!     Leave a comment  Posted in OneMillionTrees      Join the NUS Toddycats’ Battle of Pasir Panjang Commemorative Walk on Sat 3rd or 17th Feb 2024  Posted on Saturday, 20 January 2024 by otterman | 1 comment   NUS Toddycats has conducted the Battle of Pasir Panjang Commemorative Walk since 2002. During the walk, we remember the battle and also share other stories of nature, history and the environment.  Event details:  Date: Sat 3rd Feb 2024 (50 pax) or 17th Feb 2024 (30 pax) Time: 8.00am – 11.30am Register for the walk individually on EventBrite at hRequest unsuRequest unsu</t>
+        </is>
+      </c>
     </row>
     <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="A31" s="1" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>TeamSeagrass</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="C31" t="inlineStr">
         <is>
           <t>Led by a small volunteer management team, TeamSeagrass currently has about 200 volunteers from all walks of life that regularly monitor the seagrasses on Singapore's shores.</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+      <c r="D31" t="inlineStr">
         <is>
           <t>To raise awareness on the importance of seagrass meadows, threats to them, what happens if we lose them.</t>
         </is>
       </c>
-      <c r="D31" t="inlineStr">
+      <c r="E31" t="inlineStr">
         <is>
           <t>- seagrass monitoring
 - outreach</t>
         </is>
       </c>
-      <c r="E31" t="inlineStr"/>
-      <c r="F31" t="inlineStr">
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
         <is>
           <t>Yes - governments</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
+      <c r="H31" t="inlineStr">
         <is>
           <t>Mitigation/ Advocacy</t>
         </is>
       </c>
-      <c r="H31" t="inlineStr"/>
-      <c r="I31" t="inlineStr">
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K31" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/TeamSeagrass-172603406103907/', 'https://www.instagram.com/teamseagrass/', 'https://twitter.com/teamseagrass', 'https://www.flickr.com/groups/1047086@N21/']</t>
         </is>
       </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>['https://www.nparks.gov.sg/biodiversity/community-in-nature-initiative/seagrass-monitoring-by-teamseagrass', 'https://teamseagrass.blogspot.com/', 'https://teamseagrass.blogspot.com/p/faqs.html']</t>
+        </is>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">        
+ 	Seagrass Monitoring by TeamSeaGrass - Community in Nature Initiative  - Biodiversity - National Parks Board (NParks)
+                                        A Singapore Government Agency Website      Click logo to go back to the homepage   Menu        Services   Development Plan Submission   News   Contact Us   Feedback and Enquiry   E newsletter   FAQs   Sitemap        Logo to go back to the homepage     Gardens, Parks &amp; Nature
+                               Parks &amp; Nature Reserves      Park Connector Network      Nature Park Network &amp; Nature Corridors      Heritage Trees       Heritage Tree Care Guide     Heritage Tree Panel     Heritage Tree Nomination Form      Heritage Roads      Nature Ways      Therapeutic Gardens       Research and Design Guidelines     How to start a Therapeutic Garden     Therapeutic Horticulture Programmes     How to                 teamseagrass                                                                                            Pages    Home   FAQs   What are seagrasses?   dates   locations   trip preparations   Join the Team!                                                                           Feb 24, 2019      16 Mar (Sat): TeamSeagrass joins Celebrating Singapore Shores at Berlayar Creek      Save the date! A chance to win plenty of great prizes! Join fun games as TeamSeaGrass volunteers share about Singapore's seagrass and the important role they play in our marine ecosystem.    The event is FREE, no registration required. Specially for                teamseagrass: FAQs                                                                                         Pages    Home   FAQs   What are seagrasses?   dates   locations   trip preparations   Join the Team!                                                                                FAQs      What is TeamSeagrass? Led by a small volunteer management team, TeamSeagrass currently has about 200 volunteers from all walks of life that regularly monitor the seagrasses on Singapore's shores. Started in 2007, TeamSeagrass is a collaboration with the National Biodiversity Centre of the National Parks Board and international Seagrass-Watch, the largest scientific, non-destructive, seagrass assessment and monitoring program in the world.  Why study seagrasses in Singapore? Watching grass grow may seem dead boring, but it's fascinating when it's Grasses of the Sea! S</t>
+        </is>
+      </c>
     </row>
     <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="A32" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
         <is>
           <t>Singapore Blue Plan 2018</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>The Blue Plan is a ground-up initiative that presents the vision of the marine community in Singapore. The Singapore Blue Plan 2018, is the third instalment of the Blue Plan, that is presented to governments every decade.</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>a) To present the current status of coastal and marine ecosystems in Singapore
 b) To showcase the biodiversity within these ecosystems;
@@ -2250,112 +2724,128 @@
 d) To recommend measures to protect coastal and marine ecosystems into the next decade.</t>
         </is>
       </c>
-      <c r="D32" t="inlineStr">
+      <c r="E32" t="inlineStr">
         <is>
           <t>- singapore blue plan
 - symposium</t>
         </is>
       </c>
-      <c r="E32" t="inlineStr"/>
-      <c r="F32" t="inlineStr">
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr">
         <is>
           <t>Yes - governments</t>
         </is>
       </c>
-      <c r="G32" t="inlineStr">
+      <c r="H32" t="inlineStr">
         <is>
           <t>Mitigation/ Advocacy</t>
         </is>
       </c>
-      <c r="H32" t="n">
+      <c r="I32" t="n">
         <v>4</v>
       </c>
-      <c r="I32" t="inlineStr">
+      <c r="J32" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K32" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/CelebratingSingaporeShores/photos/a.1455903627838641/1922422557853410/?type=3']</t>
         </is>
       </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>['https://singaporeblueplan2018.blogspot.com/', 'https://sibiol.org.sg/wp-content/uploads/2020/10/The_Singapore_Blue_Plan_2018.pdf', 'https://coralreef.nus.edu.sg/publications/Jaafar2018.pdf']</t>
+        </is>
+      </c>
     </row>
     <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
         <is>
           <t>Herpetological Society Singapore (HSS)</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="C33" t="inlineStr">
         <is>
           <t>The Herpetological Society of Singapore is a group of herpetology enthusiasts based in Singapore. We believe in ethics, rigour and outreach.</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
+      <c r="D33" t="inlineStr">
         <is>
           <t>The Herpetological Society of Singapore is a volunteer-run group of herpetology enthusiasts. We are passionate about the conservation, appreciation, and study of reptiles and amphibians in Singapore and Southeast Asia.</t>
         </is>
       </c>
-      <c r="D33" t="inlineStr">
+      <c r="E33" t="inlineStr">
         <is>
           <t>- Herptile Roadkill Project
 - Education
 - Outreach</t>
         </is>
       </c>
-      <c r="E33" t="inlineStr"/>
-      <c r="F33" t="inlineStr">
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G33" t="inlineStr">
+      <c r="H33" t="inlineStr">
         <is>
           <t>Advocacy</t>
         </is>
       </c>
-      <c r="H33" t="n">
+      <c r="I33" t="n">
         <v>6</v>
       </c>
-      <c r="I33" t="inlineStr">
+      <c r="J33" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K33" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
           <t>['https://www.instagram.com/herpsocsg/?hl=en', 'https://www.facebook.com/herpsocsg/', 'https://www.instagram.com/herpsocsg/reels/']</t>
         </is>
       </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>['https://herpsocsg.com/', 'https://herpsocsg.com/meet-the-team/', 'https://herpsocsg.wordpress.com/']</t>
+        </is>
+      </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
         <is>
           <t>Celebrating Singapore Shores</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="C34" t="inlineStr">
         <is>
           <t>It is a community platform that brings together the Singapore marine community. This community-driven initiative brings together partners such as government agencies, NGOs, interest groups, academics, private organisations, and civil society. Started as we joined in the celebrations of International Year of the Reef 2018, Celebrating Singapore Shores goes on after 2018!</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="D34" t="inlineStr">
         <is>
           <t>This platform is to celebrate all our shores: from mangroves to seagrasses, rocky shores to reefs, even our living artificial shores!</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="E34" t="inlineStr">
         <is>
           <t>- Singapore Blue Plan 2018
 - Chek Jawa walk
@@ -2363,101 +2853,117 @@
 - Outreach Talks</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr"/>
-      <c r="F34" t="inlineStr">
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr">
         <is>
           <t>Yes - governments</t>
         </is>
       </c>
-      <c r="G34" t="inlineStr">
+      <c r="H34" t="inlineStr">
         <is>
           <t>Advocacy</t>
         </is>
       </c>
-      <c r="H34" t="inlineStr"/>
-      <c r="I34" t="inlineStr">
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr">
         <is>
           <t xml:space="preserve">Singapore </t>
         </is>
       </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K34" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/CelebratingSingaporeShores/', 'https://www.instagram.com/singaporeshores/?hl=en', 'https://www.flickr.com/groups/3147013@N21/', 'https://www.facebook.com/CelebratingSingaporeShores/videos/save-the-date-were-celebrating-singapores-shores-on-16-march-2019-from-berlayar-/2189389394705307/']</t>
         </is>
       </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>['https://celebratingsingaporeshores.blogspot.com/', 'https://celebratingsingaporeshores.blogspot.com/p/about-us.html', 'https://singapores-green-lobang.fandom.com/wiki/Celebrating_Singapore_Shores']</t>
+        </is>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>Save That Pen</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>Save That Pen gives used and unwanted pens a new lease of life. We collect donated pens from around Singapore, refill them, and pass them on to underprivileged students in Singapore and the region.</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>Give your pen a second life. Save that pen.</t>
         </is>
       </c>
-      <c r="D35" t="inlineStr">
+      <c r="E35" t="inlineStr">
         <is>
           <t>- Sort and refill pens
 - Recycle and upcycle remaining pens</t>
         </is>
       </c>
-      <c r="E35" t="inlineStr"/>
-      <c r="F35" t="inlineStr">
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr">
         <is>
           <t>Yes - businesses</t>
         </is>
       </c>
-      <c r="G35" t="inlineStr">
+      <c r="H35" t="inlineStr">
         <is>
           <t>Adaptation</t>
         </is>
       </c>
-      <c r="H35" t="inlineStr"/>
-      <c r="I35" t="inlineStr">
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J35" t="inlineStr">
+      <c r="K35" t="inlineStr">
         <is>
           <t>SIngaporean</t>
         </is>
       </c>
-      <c r="K35" t="inlineStr">
+      <c r="L35" t="inlineStr">
         <is>
           <t>['https://www.facebook.com/SaveThatPen/']</t>
         </is>
       </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>['https://www.savethatpen.org/', 'https://www.savethatpen.org/about', 'https://www.ntuc.org.sg/youngntuc/about-us/affinity-groups/save-that-pen']</t>
+        </is>
+      </c>
     </row>
     <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
         <is>
           <t>ACRES (Animal Concerns Research and Education Society)</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="C36" t="inlineStr">
         <is>
           <t>ACRES strives to create a kind and compassionate society towards all life, through humane education, promoting cruelty-free lifestyle, 24-hr wildlife rescue services, tackling the illegal wildlife trade and providing a home for rescued illegally trafficked wildlife in Singapore.</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+      <c r="D36" t="inlineStr">
         <is>
           <t>To create a caring and socially responsible society where animals are treated as sentient beings.</t>
         </is>
       </c>
-      <c r="D36" t="inlineStr">
+      <c r="E36" t="inlineStr">
         <is>
           <t>- Promoting coexistence with Singapore's wildlife
 - Conducting roadshows
@@ -2467,58 +2973,66 @@
 - Working together with the TCM industry on the ACRES and STOC Endangered-Species Friendly Labelling Scheme</t>
         </is>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>- Grants 
 - Donations</t>
         </is>
       </c>
-      <c r="F36" t="inlineStr">
+      <c r="G36" t="inlineStr">
         <is>
           <t>Yes - governments and businesses</t>
         </is>
       </c>
-      <c r="G36" t="inlineStr">
+      <c r="H36" t="inlineStr">
         <is>
           <t>Adaptation</t>
         </is>
       </c>
-      <c r="H36" t="n">
+      <c r="I36" t="n">
         <v>21</v>
       </c>
-      <c r="I36" t="inlineStr">
+      <c r="J36" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K36" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/ACRESasia/', 'https://sg.linkedin.com/company/acressg', 'https://www.facebook.com/ACRESasia/photos/']</t>
         </is>
       </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>['https://acres.org.sg/', 'https://en.wikipedia.org/wiki/Animal_Concerns_Research_and_Education_Society', 'https://www.devex.com/organizations/animal-concerns-research-education-society-acres-49497']</t>
+        </is>
+      </c>
     </row>
     <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>Little Green Men</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="C37" t="inlineStr">
         <is>
           <t>Little Green Men Singapore (LGM) is a non-profit initiative by Sarah, Sue-Ann, and Frances, who want to do good for the environment. We had humble beginnings in June 2016, realising that the people around us didn’t see and didn’t care for how their actions, choices, and lifestyles affected the environment. How could people care for something they didn’t know?</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+      <c r="D37" t="inlineStr">
         <is>
           <t>Enabling regular folks to interact more with nature and see how it pervades every aspect of our lives</t>
         </is>
       </c>
-      <c r="D37" t="inlineStr">
+      <c r="E37" t="inlineStr">
         <is>
           <t>Coastal clean ups (Chek Jawa, Sungei Tampines, Lim Chu Kang, Sungei Pandan, Sungei Seletar, Sungei Buloh Wetland Reserve)
 Nature walks (Lentor Forest, Green Corridor, Tengah Forest, Windsor Nature Park, Jurong Lake Gardens, Thomson Nature Park)
@@ -2527,53 +3041,61 @@
 Film screening (Wasted! The Story of Food Waste)</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr"/>
-      <c r="F37" t="inlineStr">
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
+      <c r="H37" t="inlineStr">
         <is>
           <t>Mitigation/ Advocacy</t>
         </is>
       </c>
-      <c r="H37" t="n">
+      <c r="I37" t="n">
         <v>3</v>
       </c>
-      <c r="I37" t="inlineStr">
+      <c r="J37" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K37" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/littlegreenmensg/', 'https://www.instagram.com/littlegreenmensg/?hl=en']</t>
         </is>
       </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>['https://en.wikipedia.org/wiki/Little_green_men_(Russo-Ukrainian_War)', 'https://en.wikipedia.org/wiki/Little_green_men', 'https://littlegreenmensg.wordpress.com/']</t>
+        </is>
+      </c>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>SG Food Rescue</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>We reduce food waste in Singapore by transforming people’s mindsets about food waste through our activities. These include our food rescue programmes, where we approach businesses and ask them not to throw food away, and instead give it to us who pass it on to those who can use it.</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t xml:space="preserve">Rescue food and reduce food waste </t>
         </is>
       </c>
-      <c r="D38" t="inlineStr">
+      <c r="E38" t="inlineStr">
         <is>
           <t>- Veggie Rescue @ Pasir Panjang
 - Veggie Collection
@@ -2582,51 +3104,59 @@
 - Talks</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>- Donations
 - Sponsorships</t>
         </is>
       </c>
-      <c r="F38" t="inlineStr">
+      <c r="G38" t="inlineStr">
         <is>
           <t>Yes - businesses</t>
         </is>
       </c>
-      <c r="G38" t="inlineStr">
+      <c r="H38" t="inlineStr">
         <is>
           <t>Mitigation</t>
         </is>
       </c>
-      <c r="H38" t="inlineStr"/>
-      <c r="I38" t="inlineStr">
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K38" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/groups/sgfoodrescue/', 'https://www.facebook.com/foodrescuesingapore/', 'https://www.instagram.com/sgfoodrescue/?hl=en']</t>
         </is>
       </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>['https://sgfoodrescue.wordpress.com/', 'https://www.sg/stories/imperfectly-edible', 'https://sgfoodrescue.wordpress.com/operations/']</t>
+        </is>
+      </c>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
         <is>
           <t>NUS SAVE (Students' Association for Visions of the Earth)</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="C39" t="inlineStr">
         <is>
           <t>NUS SAVE is the leading environmental group on campus. We work with fellow students, school offices and various other stakeholders to inspire a greener NUS. Through our self-led initiatives, we advocate for NUS to be an exemplary model in the areas of sustainability and climate action.</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+      <c r="D39" t="inlineStr">
         <is>
           <t>- To inspire behavioural change through meaningful and sustainable initiatives
 - To create accessible, visible, and attractive eco-friendly choices for the NUS community
@@ -2635,7 +3165,7 @@
 - To effect purposeful structural change to address the current climate crisis</t>
         </is>
       </c>
-      <c r="D39" t="inlineStr">
+      <c r="E39" t="inlineStr">
         <is>
           <t>- Guided Nature Walks
 - Beach Cleanup at Sembawang Park
@@ -2651,108 +3181,124 @@
 - Upcycling Education</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>- Partnerships</t>
         </is>
       </c>
-      <c r="F39" t="inlineStr">
+      <c r="G39" t="inlineStr">
         <is>
           <t xml:space="preserve">Yes - businesses </t>
         </is>
       </c>
-      <c r="G39" t="inlineStr">
+      <c r="H39" t="inlineStr">
         <is>
           <t>Mitigation/ Advocacy</t>
         </is>
       </c>
-      <c r="H39" t="inlineStr">
+      <c r="I39" t="inlineStr">
         <is>
           <t>30+</t>
         </is>
       </c>
-      <c r="I39" t="inlineStr">
+      <c r="J39" t="inlineStr">
         <is>
           <t xml:space="preserve">Singapore </t>
         </is>
       </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K39" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
           <t>['https://www.instagram.com/nussave/', 'https://www.facebook.com/NUSSAVE/', 'https://sg.linkedin.com/company/nussave', 'https://www.instagram.com/nussave/reels/']</t>
         </is>
       </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>['https://nussavewrites.wordpress.com/', 'https://sustainability.nus.edu.sg/get-involved/environmental-student-groups/', 'https://nussavewrites.wordpress.com/our-story/']</t>
+        </is>
+      </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
         <is>
           <t>Eco-SIM</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="C40" t="inlineStr">
         <is>
           <t>Founded in 2017, Eco-SIM is a student-led environmental group that serves to bridge the gap between students and the natural environment. The club encourages individuals to take more responsibility and action in their roles as custodians of the Earth. Activities conducted by Eco-SIM includes sustainability fair, hullabaloo, visiting various sites as well as other environmentally friendly initiatives.</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="D40" t="inlineStr">
         <is>
           <t>encourages individuals to take more responsibility and action in their roles as custodians of the Earth</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="E40" t="inlineStr">
         <is>
           <t>- Sustainability Fairs</t>
         </is>
       </c>
-      <c r="E40" t="inlineStr"/>
-      <c r="F40" t="inlineStr">
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr">
         <is>
           <t>Yes - businesses</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="H40" t="inlineStr">
         <is>
           <t>Mitigation/ Advocacy</t>
         </is>
       </c>
-      <c r="H40" t="inlineStr"/>
-      <c r="I40" t="inlineStr">
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr">
         <is>
           <t xml:space="preserve">Singapore </t>
         </is>
       </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K40" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
           <t>['https://sg.linkedin.com/company/eco-sim', 'https://www.facebook.com/EcoSIMClub/']</t>
         </is>
       </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>['https://project1095.simge.edu.sg/student-life/special-interest-clubs/sim-eco-sim/', 'https://www.thalesgroup.com/en/markets/digital-identity-and-security/mobile/secure-elements/eco-sim', 'https://www.m1.com.sg/about-us/news-releases/2023/m1-eco-sim']</t>
+        </is>
+      </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
         <is>
           <t>Environmental Law Students' Association (ELSA)</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>The Environmental Law Students’ Association (ELSA) is an NUS Law interest group affiliated with the Asia-Pacific Centre for Environmental Law (APCEL). Founded in 2016, ELSA seeks to become the undergraduate centre in environmental law and policy, anchored in Singapore but with a continuing interest in Southeast Asia and the wider Asia-Pacific region.</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>Our substantive focus is on Singapore environment and land use law. Guided by the overarching principle of intergenerational environmental justice, we encourage students to get involved in environmental law and policy.</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="E41" t="inlineStr">
         <is>
           <t>- Sustainability+ dialogue
 - Singapore Botanic Gardens Trails
@@ -2760,53 +3306,61 @@
 - Research</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr"/>
-      <c r="F41" t="inlineStr">
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G41" t="inlineStr">
+      <c r="H41" t="inlineStr">
         <is>
           <t>Mitigation/ Advocacy</t>
         </is>
       </c>
-      <c r="H41" t="n">
+      <c r="I41" t="n">
         <v>9</v>
       </c>
-      <c r="I41" t="inlineStr">
+      <c r="J41" t="inlineStr">
         <is>
           <t xml:space="preserve">Singaproe </t>
         </is>
       </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K41" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
           <t>['https://sg.linkedin.com/company/elsa-nuslaw', 'https://www.instagram.com/nuslawelsa/', 'https://www.facebook.com/elsa.nuslaw/', 'https://www.facebook.com/elsaualberta/', 'https://www.instagram.com/uottawaelsa/?hl=en']</t>
         </is>
       </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>['https://www.elsauottawa.org/', 'https://elsa.org/', 'https://www.elsauottawa.org/about']</t>
+        </is>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>NUS Vision of Equality for a Greener Earth</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="C42" t="inlineStr">
         <is>
           <t>Vision of Equality for a Greener Earth (VEGE) is a student organisation in NUS that champions the plant-based movement.</t>
         </is>
       </c>
-      <c r="C42" t="inlineStr">
+      <c r="D42" t="inlineStr">
         <is>
           <t>To raise the awareness of the moral and environmental aspects of a plant-based diet through education and empower students to initiate projects to accelerate this change.</t>
         </is>
       </c>
-      <c r="D42" t="inlineStr">
+      <c r="E42" t="inlineStr">
         <is>
           <t>- vegan potlucks
 - food tours
@@ -2814,51 +3368,59 @@
 - other projects, and creating roles for members to concurrently contribute to the plant-based movement</t>
         </is>
       </c>
-      <c r="E42" t="inlineStr"/>
-      <c r="F42" t="inlineStr">
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="G42" t="inlineStr">
+      <c r="H42" t="inlineStr">
         <is>
           <t>Mitigation/ Advocacy</t>
         </is>
       </c>
-      <c r="H42" t="inlineStr"/>
-      <c r="I42" t="inlineStr">
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K42" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
           <t>['https://www.facebook.com/nusvege/', 'https://www.instagram.com/nusvege/?hl=en']</t>
         </is>
       </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>['https://sustainability.nus.edu.sg/get-involved/environmental-student-groups/#:~:text=Vision%20of%20Equality%20for%20a,champions%20the%20plant%2Dbased%20movement.', 'https://nus.campuslabs.com/engage/organization/vege', 'https://news.nus.edu.sg/save-the-earth-starting-from-your-plate/']</t>
+        </is>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" t="inlineStr">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
         <is>
           <t>Earthlink NTU</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
+      <c r="C43" t="inlineStr">
         <is>
           <t>Since 1993, Earthlink has led NTU’s environmental activities. Here, passionate individuals with a vision for a healthier planet plan outreach events and activities to raise awareness for environmental issues. To cover the diverse categories that can range from nature appreciation to going plastic-lite to eating less meat, Earthlink has fifteen portfolios organised under four broad Committees of Campaigns, Events, Operations and Projects.</t>
         </is>
       </c>
-      <c r="C43" t="inlineStr">
+      <c r="D43" t="inlineStr">
         <is>
           <t>Raise awareness of environmental issues</t>
         </is>
       </c>
-      <c r="D43" t="inlineStr">
+      <c r="E43" t="inlineStr">
         <is>
           <t>- Guided tours
 - NTU Biodiversity Week
@@ -2867,31 +3429,36 @@
 - EcoVenture</t>
         </is>
       </c>
-      <c r="E43" t="inlineStr"/>
-      <c r="F43" t="inlineStr">
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr">
         <is>
           <t>Yes - businesses</t>
         </is>
       </c>
-      <c r="G43" t="inlineStr">
+      <c r="H43" t="inlineStr">
         <is>
           <t>Mitigation/ Advocacy</t>
         </is>
       </c>
-      <c r="H43" t="inlineStr"/>
-      <c r="I43" t="inlineStr">
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr">
         <is>
           <t>Singapore</t>
         </is>
       </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>Singaporean</t>
-        </is>
-      </c>
       <c r="K43" t="inlineStr">
         <is>
+          <t>Singaporean</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
           <t>['https://www.instagram.com/earthlinkntu/?hl=en', 'https://sg.linkedin.com/company/earthlink-ntu', 'https://www.facebook.com/earthlinkntu/', 'https://twitter.com/earthlinkntu?lang=en', 'https://www.facebook.com/EarthlinkNTUsg/']</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>['https://blogs.ntu.edu.sg/sao-earthlinkntu/', 'https://blogs.ntu.edu.sg/colab4good/tag/earthlink-ntu/', 'https://singapores-green-lobang.fandom.com/wiki/Earthlink_NTU']</t>
         </is>
       </c>
     </row>

</xml_diff>